<commit_message>
Gruppe E: Auswahl der umzusetzenden Funktionen
"wird erledigt"
</commit_message>
<xml_diff>
--- a/mgmt/Funktionsliste-Teamaufteilung.xlsx
+++ b/mgmt/Funktionsliste-Teamaufteilung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hspforzheimde-my.sharepoint.com/personal/staibflo_hs-pforzheim_de/Documents/für HS/SE/GitHub/excelator/mgmt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{BD76375E-882C-934F-8082-3697347F1EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3773E9DA-EBD6-4440-A99B-5B3AFAB16E64}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{BD76375E-882C-934F-8082-3697347F1EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16C63939-05ED-4E9C-86A2-7B8FCBEAF6BC}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{1F02C744-EE90-A14B-9229-2ACDAC5D761E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1982" uniqueCount="1131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1989" uniqueCount="1133">
   <si>
     <t>Funktionsname</t>
   </si>
@@ -9411,6 +9411,12 @@
   </si>
   <si>
     <t>Kategorie</t>
+  </si>
+  <si>
+    <t>wird umgesetzt</t>
+  </si>
+  <si>
+    <t>&amp;</t>
   </si>
 </sst>
 </file>
@@ -9515,7 +9521,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -9546,14 +9552,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9561,32 +9561,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF1E1E1E"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -9653,6 +9627,32 @@
         <scheme val="minor"/>
       </font>
       <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF1E1E1E"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -9727,6 +9727,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C418F1F6-3AF5-EF4E-8CE1-8CA525105B91}" name="Tabelle1" displayName="Tabelle1" ref="A1:H505" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A1:H505" xr:uid="{C418F1F6-3AF5-EF4E-8CE1-8CA525105B91}"/>
@@ -9736,14 +9740,14 @@
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{10428CB8-DF17-C24D-A8C2-8B4827E181B0}" name="Funktionsname" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{98C1F64B-509E-934D-BBC9-297E60C938D9}" name="Team" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{CCBD6B5F-84D2-495B-9B03-9C5B7B0ADD01}" name="Kategorie" dataDxfId="0">
+    <tableColumn id="8" xr3:uid="{CCBD6B5F-84D2-495B-9B03-9C5B7B0ADD01}" name="Kategorie" dataDxfId="5">
       <calculatedColumnFormula>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{58872452-BA7B-944C-9D5A-2F8DFEAA42D8}" name="Beschreibung" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{C34E4242-AD8F-C049-A8FD-DE3980EA15A5}" name="Schon Implementiert (Funktionsname in Excelator)" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{47391C81-2EA8-A148-8D5A-099836562F33}" name="Status" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{E7210489-D250-D545-A3A7-8B64CF95D33B}" name="Kommentar" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{2FB03DEE-9D86-E448-AC9D-37A85488B243}" name="Nicht möglich" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{58872452-BA7B-944C-9D5A-2F8DFEAA42D8}" name="Beschreibung" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{C34E4242-AD8F-C049-A8FD-DE3980EA15A5}" name="Schon Implementiert (Funktionsname in Excelator)" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{47391C81-2EA8-A148-8D5A-099836562F33}" name="Status" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{E7210489-D250-D545-A3A7-8B64CF95D33B}" name="Kommentar" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{2FB03DEE-9D86-E448-AC9D-37A85488B243}" name="Nicht möglich" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -10048,9 +10052,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9E696CC-4DD8-8E43-8BCC-2210EBDA2D24}">
   <dimension ref="A1:J505"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="57" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A486" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A465" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -18564,7 +18568,7 @@
       </c>
       <c r="E410" s="8"/>
       <c r="F410" s="8"/>
-      <c r="G410" s="12"/>
+      <c r="G410" s="8"/>
       <c r="H410" s="8" t="s">
         <v>1016</v>
       </c>
@@ -18585,7 +18589,7 @@
       </c>
       <c r="E411" s="8"/>
       <c r="F411" s="8"/>
-      <c r="G411" s="12"/>
+      <c r="G411" s="8"/>
       <c r="H411" s="8" t="s">
         <v>1016</v>
       </c>
@@ -18606,7 +18610,7 @@
       </c>
       <c r="E412" s="8"/>
       <c r="F412" s="8"/>
-      <c r="G412" s="12"/>
+      <c r="G412" s="8"/>
       <c r="H412" s="8" t="s">
         <v>1016</v>
       </c>
@@ -18627,7 +18631,7 @@
       </c>
       <c r="E413" s="8"/>
       <c r="F413" s="8"/>
-      <c r="G413" s="12"/>
+      <c r="G413" s="8"/>
       <c r="H413" s="8" t="s">
         <v>1016</v>
       </c>
@@ -18648,7 +18652,7 @@
       </c>
       <c r="E414" s="8"/>
       <c r="F414" s="8"/>
-      <c r="G414" s="12"/>
+      <c r="G414" s="8"/>
       <c r="H414" s="8" t="s">
         <v>1016</v>
       </c>
@@ -18669,7 +18673,7 @@
       </c>
       <c r="E415" s="8"/>
       <c r="F415" s="8"/>
-      <c r="G415" s="12"/>
+      <c r="G415" s="8"/>
       <c r="H415" s="8" t="s">
         <v>1016</v>
       </c>
@@ -18690,7 +18694,7 @@
       </c>
       <c r="E416" s="8"/>
       <c r="F416" s="8"/>
-      <c r="G416" s="12"/>
+      <c r="G416" s="8"/>
       <c r="H416" s="8" t="s">
         <v>1016</v>
       </c>
@@ -18711,7 +18715,7 @@
       </c>
       <c r="E417" s="8"/>
       <c r="F417" s="8"/>
-      <c r="G417" s="12"/>
+      <c r="G417" s="8"/>
       <c r="H417" s="8" t="s">
         <v>1016</v>
       </c>
@@ -18732,7 +18736,7 @@
       </c>
       <c r="E418" s="8"/>
       <c r="F418" s="8"/>
-      <c r="G418" s="12"/>
+      <c r="G418" s="8"/>
       <c r="H418" s="8" t="s">
         <v>1016</v>
       </c>
@@ -18753,7 +18757,7 @@
       </c>
       <c r="E419" s="8"/>
       <c r="F419" s="8"/>
-      <c r="G419" s="12"/>
+      <c r="G419" s="8"/>
       <c r="H419" s="8" t="s">
         <v>1016</v>
       </c>
@@ -18774,7 +18778,7 @@
       </c>
       <c r="E420" s="8"/>
       <c r="F420" s="8"/>
-      <c r="G420" s="12" t="s">
+      <c r="G420" s="8" t="s">
         <v>1078</v>
       </c>
       <c r="H420" s="8"/>
@@ -18795,7 +18799,7 @@
       </c>
       <c r="E421" s="8"/>
       <c r="F421" s="8"/>
-      <c r="G421" s="12"/>
+      <c r="G421" s="8"/>
       <c r="H421" s="8" t="s">
         <v>1016</v>
       </c>
@@ -18816,7 +18820,7 @@
       </c>
       <c r="E422" s="8"/>
       <c r="F422" s="8"/>
-      <c r="G422" s="12"/>
+      <c r="G422" s="8"/>
       <c r="H422" s="8" t="s">
         <v>1016</v>
       </c>
@@ -18837,7 +18841,7 @@
       </c>
       <c r="E423" s="8"/>
       <c r="F423" s="8"/>
-      <c r="G423" s="12" t="s">
+      <c r="G423" s="8" t="s">
         <v>1079</v>
       </c>
       <c r="H423" s="8"/>
@@ -18858,12 +18862,12 @@
       </c>
       <c r="E424" s="8"/>
       <c r="F424" s="8"/>
-      <c r="G424" s="12" t="s">
+      <c r="G424" s="8" t="s">
         <v>1080</v>
       </c>
       <c r="H424" s="8"/>
     </row>
-    <row r="425" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="425" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A425" s="6" t="s">
         <v>12</v>
       </c>
@@ -18877,11 +18881,11 @@
       <c r="D425" s="7" t="s">
         <v>923</v>
       </c>
-      <c r="E425" s="8"/>
+      <c r="E425" s="8" t="s">
+        <v>1132</v>
+      </c>
       <c r="F425" s="8"/>
-      <c r="G425" s="12" t="s">
-        <v>1080</v>
-      </c>
+      <c r="G425" s="8"/>
       <c r="H425" s="8"/>
     </row>
     <row r="426" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
@@ -18899,8 +18903,10 @@
         <v>924</v>
       </c>
       <c r="E426" s="8"/>
-      <c r="F426" s="8"/>
-      <c r="G426" s="12" t="s">
+      <c r="F426" s="8" t="s">
+        <v>1131</v>
+      </c>
+      <c r="G426" s="8" t="s">
         <v>1080</v>
       </c>
       <c r="H426" s="8"/>
@@ -18921,7 +18927,7 @@
       </c>
       <c r="E427" s="8"/>
       <c r="F427" s="8"/>
-      <c r="G427" s="12"/>
+      <c r="G427" s="8"/>
       <c r="H427" s="8" t="s">
         <v>1016</v>
       </c>
@@ -18942,7 +18948,7 @@
       </c>
       <c r="E428" s="8"/>
       <c r="F428" s="8"/>
-      <c r="G428" s="12"/>
+      <c r="G428" s="8"/>
       <c r="H428" s="8" t="s">
         <v>1016</v>
       </c>
@@ -18963,7 +18969,7 @@
       </c>
       <c r="E429" s="8"/>
       <c r="F429" s="8"/>
-      <c r="G429" s="12"/>
+      <c r="G429" s="8"/>
       <c r="H429" s="8" t="s">
         <v>1016</v>
       </c>
@@ -18984,7 +18990,7 @@
       </c>
       <c r="E430" s="8"/>
       <c r="F430" s="8"/>
-      <c r="G430" s="12"/>
+      <c r="G430" s="8"/>
       <c r="H430" s="8" t="s">
         <v>1016</v>
       </c>
@@ -19005,7 +19011,7 @@
       </c>
       <c r="E431" s="8"/>
       <c r="F431" s="8"/>
-      <c r="G431" s="12"/>
+      <c r="G431" s="8"/>
       <c r="H431" s="8" t="s">
         <v>1016</v>
       </c>
@@ -19026,7 +19032,7 @@
       </c>
       <c r="E432" s="8"/>
       <c r="F432" s="8"/>
-      <c r="G432" s="12"/>
+      <c r="G432" s="8"/>
       <c r="H432" s="8" t="s">
         <v>1016</v>
       </c>
@@ -19047,7 +19053,7 @@
       </c>
       <c r="E433" s="8"/>
       <c r="F433" s="8"/>
-      <c r="G433" s="12" t="s">
+      <c r="G433" s="8" t="s">
         <v>1080</v>
       </c>
       <c r="H433" s="8"/>
@@ -19068,7 +19074,7 @@
       </c>
       <c r="E434" s="8"/>
       <c r="F434" s="8"/>
-      <c r="G434" s="12" t="s">
+      <c r="G434" s="8" t="s">
         <v>1080</v>
       </c>
       <c r="H434" s="8"/>
@@ -19089,7 +19095,7 @@
       </c>
       <c r="E435" s="8"/>
       <c r="F435" s="8"/>
-      <c r="G435" s="12" t="s">
+      <c r="G435" s="8" t="s">
         <v>1080</v>
       </c>
       <c r="H435" s="8"/>
@@ -19112,7 +19118,7 @@
         <v>1081</v>
       </c>
       <c r="F436" s="8"/>
-      <c r="G436" s="12"/>
+      <c r="G436" s="8"/>
       <c r="H436" s="8"/>
     </row>
     <row r="437" spans="1:8" x14ac:dyDescent="0.5">
@@ -19131,7 +19137,7 @@
       </c>
       <c r="E437" s="8"/>
       <c r="F437" s="8"/>
-      <c r="G437" s="12"/>
+      <c r="G437" s="8"/>
       <c r="H437" s="8" t="s">
         <v>1016</v>
       </c>
@@ -19154,7 +19160,7 @@
         <v>1081</v>
       </c>
       <c r="F438" s="8"/>
-      <c r="G438" s="12"/>
+      <c r="G438" s="8"/>
       <c r="H438" s="8"/>
     </row>
     <row r="439" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
@@ -19173,7 +19179,7 @@
       </c>
       <c r="E439" s="8"/>
       <c r="F439" s="8"/>
-      <c r="G439" s="12"/>
+      <c r="G439" s="8"/>
       <c r="H439" s="8" t="s">
         <v>1016</v>
       </c>
@@ -19194,7 +19200,7 @@
       </c>
       <c r="E440" s="8"/>
       <c r="F440" s="8"/>
-      <c r="G440" s="12"/>
+      <c r="G440" s="8"/>
       <c r="H440" s="8" t="s">
         <v>1016</v>
       </c>
@@ -19215,7 +19221,7 @@
       </c>
       <c r="E441" s="8"/>
       <c r="F441" s="8"/>
-      <c r="G441" s="12"/>
+      <c r="G441" s="8"/>
       <c r="H441" s="8" t="s">
         <v>1016</v>
       </c>
@@ -19236,7 +19242,7 @@
       </c>
       <c r="E442" s="8"/>
       <c r="F442" s="8"/>
-      <c r="G442" s="12"/>
+      <c r="G442" s="8"/>
       <c r="H442" s="8" t="s">
         <v>1016</v>
       </c>
@@ -19257,7 +19263,7 @@
       </c>
       <c r="E443" s="8"/>
       <c r="F443" s="8"/>
-      <c r="G443" s="12"/>
+      <c r="G443" s="8"/>
       <c r="H443" s="8" t="s">
         <v>1016</v>
       </c>
@@ -19278,7 +19284,7 @@
       </c>
       <c r="E444" s="8"/>
       <c r="F444" s="8"/>
-      <c r="G444" s="12" t="s">
+      <c r="G444" s="8" t="s">
         <v>1080</v>
       </c>
       <c r="H444" s="8"/>
@@ -19299,7 +19305,7 @@
       </c>
       <c r="E445" s="8"/>
       <c r="F445" s="8"/>
-      <c r="G445" s="12" t="s">
+      <c r="G445" s="8" t="s">
         <v>1080</v>
       </c>
       <c r="H445" s="8"/>
@@ -19320,7 +19326,7 @@
       </c>
       <c r="E446" s="8"/>
       <c r="F446" s="8"/>
-      <c r="G446" s="12"/>
+      <c r="G446" s="8"/>
       <c r="H446" s="8" t="s">
         <v>1016</v>
       </c>
@@ -19341,7 +19347,7 @@
       </c>
       <c r="E447" s="8"/>
       <c r="F447" s="8"/>
-      <c r="G447" s="12"/>
+      <c r="G447" s="8"/>
       <c r="H447" s="8" t="s">
         <v>1016</v>
       </c>
@@ -19362,7 +19368,7 @@
       </c>
       <c r="E448" s="8"/>
       <c r="F448" s="8"/>
-      <c r="G448" s="12" t="s">
+      <c r="G448" s="8" t="s">
         <v>1080</v>
       </c>
       <c r="H448" s="8"/>
@@ -19383,7 +19389,7 @@
       </c>
       <c r="E449" s="8"/>
       <c r="F449" s="8"/>
-      <c r="G449" s="12" t="s">
+      <c r="G449" s="8" t="s">
         <v>1080</v>
       </c>
       <c r="H449" s="8"/>
@@ -19404,7 +19410,7 @@
       </c>
       <c r="E450" s="8"/>
       <c r="F450" s="8"/>
-      <c r="G450" s="12" t="s">
+      <c r="G450" s="8" t="s">
         <v>1080</v>
       </c>
       <c r="H450" s="8"/>
@@ -19425,7 +19431,7 @@
       </c>
       <c r="E451" s="8"/>
       <c r="F451" s="8"/>
-      <c r="G451" s="12" t="s">
+      <c r="G451" s="8" t="s">
         <v>1082</v>
       </c>
       <c r="H451" s="8"/>
@@ -19605,7 +19611,9 @@
       <c r="E459" s="8" t="s">
         <v>1093</v>
       </c>
-      <c r="F459" s="8"/>
+      <c r="F459" s="8" t="s">
+        <v>1131</v>
+      </c>
       <c r="G459" s="8" t="s">
         <v>1129</v>
       </c>
@@ -19633,13 +19641,13 @@
       <c r="H460" s="8"/>
     </row>
     <row r="461" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A461" s="13" t="s">
+      <c r="A461" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="B461" s="14" t="s">
+      <c r="B461" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C461" s="14" t="str">
+      <c r="C461" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Logical</v>
       </c>
@@ -19654,13 +19662,13 @@
       <c r="H461" s="8"/>
     </row>
     <row r="462" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A462" s="13" t="s">
+      <c r="A462" s="12" t="s">
         <v>218</v>
       </c>
-      <c r="B462" s="14" t="s">
+      <c r="B462" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C462" s="14" t="str">
+      <c r="C462" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Logical</v>
       </c>
@@ -19675,13 +19683,13 @@
       <c r="H462" s="8"/>
     </row>
     <row r="463" spans="1:8" ht="63" x14ac:dyDescent="0.5">
-      <c r="A463" s="13" t="s">
+      <c r="A463" s="12" t="s">
         <v>473</v>
       </c>
-      <c r="B463" s="14" t="s">
+      <c r="B463" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C463" s="14" t="str">
+      <c r="C463" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Text</v>
       </c>
@@ -19698,13 +19706,13 @@
       </c>
     </row>
     <row r="464" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A464" s="13" t="s">
+      <c r="A464" s="12" t="s">
         <v>474</v>
       </c>
-      <c r="B464" s="14" t="s">
+      <c r="B464" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C464" s="14" t="str">
+      <c r="C464" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Text</v>
       </c>
@@ -19719,13 +19727,13 @@
       </c>
     </row>
     <row r="465" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A465" s="13" t="s">
+      <c r="A465" s="12" t="s">
         <v>383</v>
       </c>
-      <c r="B465" s="14" t="s">
+      <c r="B465" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C465" s="14" t="str">
+      <c r="C465" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Text</v>
       </c>
@@ -19742,13 +19750,13 @@
       </c>
     </row>
     <row r="466" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A466" s="13" t="s">
+      <c r="A466" s="12" t="s">
         <v>485</v>
       </c>
-      <c r="B466" s="14" t="s">
+      <c r="B466" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C466" s="14" t="str">
+      <c r="C466" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Date and time</v>
       </c>
@@ -19763,13 +19771,13 @@
       </c>
     </row>
     <row r="467" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A467" s="13" t="s">
+      <c r="A467" s="12" t="s">
         <v>262</v>
       </c>
-      <c r="B467" s="14" t="s">
+      <c r="B467" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C467" s="14" t="str">
+      <c r="C467" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Information</v>
       </c>
@@ -19784,13 +19792,13 @@
       </c>
     </row>
     <row r="468" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A468" s="13" t="s">
+      <c r="A468" s="12" t="s">
         <v>413</v>
       </c>
-      <c r="B468" s="14" t="s">
+      <c r="B468" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C468" s="14" t="str">
+      <c r="C468" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Math and trigonometry</v>
       </c>
@@ -19800,20 +19808,22 @@
       <c r="E468" t="s">
         <v>1086</v>
       </c>
-      <c r="F468" s="8"/>
+      <c r="F468" s="8" t="s">
+        <v>1131</v>
+      </c>
       <c r="G468" s="8" t="s">
         <v>1087</v>
       </c>
       <c r="H468" s="8"/>
     </row>
     <row r="469" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A469" s="13" t="s">
+      <c r="A469" s="12" t="s">
         <v>414</v>
       </c>
-      <c r="B469" s="14" t="s">
+      <c r="B469" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C469" s="14" t="str">
+      <c r="C469" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Math and trigonometry</v>
       </c>
@@ -19828,13 +19838,13 @@
       <c r="H469" s="8"/>
     </row>
     <row r="470" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A470" s="13" t="s">
+      <c r="A470" s="12" t="s">
         <v>209</v>
       </c>
-      <c r="B470" s="14" t="s">
+      <c r="B470" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C470" s="14" t="str">
+      <c r="C470" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Lookup and reference</v>
       </c>
@@ -19849,13 +19859,13 @@
       </c>
     </row>
     <row r="471" spans="1:8" ht="63" x14ac:dyDescent="0.5">
-      <c r="A471" s="13" t="s">
+      <c r="A471" s="12" t="s">
         <v>493</v>
       </c>
-      <c r="B471" s="14" t="s">
+      <c r="B471" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C471" s="14" t="str">
+      <c r="C471" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Financial</v>
       </c>
@@ -19872,13 +19882,13 @@
       </c>
     </row>
     <row r="472" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A472" s="13" t="s">
+      <c r="A472" s="12" t="s">
         <v>496</v>
       </c>
-      <c r="B472" s="14" t="s">
+      <c r="B472" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C472" s="14" t="str">
+      <c r="C472" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Financial</v>
       </c>
@@ -19893,13 +19903,13 @@
       </c>
     </row>
     <row r="473" spans="1:8" ht="63" x14ac:dyDescent="0.5">
-      <c r="A473" s="13" t="s">
+      <c r="A473" s="12" t="s">
         <v>494</v>
       </c>
-      <c r="B473" s="14" t="s">
+      <c r="B473" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C473" s="14" t="str">
+      <c r="C473" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Lookup and reference</v>
       </c>
@@ -19914,13 +19924,13 @@
       </c>
     </row>
     <row r="474" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A474" s="13" t="s">
+      <c r="A474" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="B474" s="14" t="s">
+      <c r="B474" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C474" s="14" t="str">
+      <c r="C474" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Web</v>
       </c>
@@ -19935,13 +19945,13 @@
       </c>
     </row>
     <row r="475" spans="1:8" ht="94.5" x14ac:dyDescent="0.5">
-      <c r="A475" s="13" t="s">
+      <c r="A475" s="12" t="s">
         <v>497</v>
       </c>
-      <c r="B475" s="14" t="s">
+      <c r="B475" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C475" s="14" t="str">
+      <c r="C475" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Logical</v>
       </c>
@@ -19949,20 +19959,22 @@
         <v>972</v>
       </c>
       <c r="E475" s="8"/>
-      <c r="F475" s="8"/>
+      <c r="F475" s="8" t="s">
+        <v>1131</v>
+      </c>
       <c r="G475" s="8" t="s">
         <v>1089</v>
       </c>
       <c r="H475" s="8"/>
     </row>
     <row r="476" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A476" s="13" t="s">
+      <c r="A476" s="12" t="s">
         <v>495</v>
       </c>
-      <c r="B476" s="14" t="s">
+      <c r="B476" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C476" s="14" t="str">
+      <c r="C476" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Lookup and reference</v>
       </c>
@@ -19977,13 +19989,13 @@
       </c>
     </row>
     <row r="477" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A477" s="13" t="s">
+      <c r="A477" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="B477" s="14" t="s">
+      <c r="B477" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C477" s="14" t="str">
+      <c r="C477" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Statistical</v>
       </c>
@@ -19998,13 +20010,13 @@
       </c>
     </row>
     <row r="478" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A478" s="13" t="s">
+      <c r="A478" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="B478" s="14" t="s">
+      <c r="B478" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C478" s="14" t="str">
+      <c r="C478" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Statistical</v>
       </c>
@@ -20019,13 +20031,13 @@
       </c>
     </row>
     <row r="479" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A479" s="13" t="s">
+      <c r="A479" s="12" t="s">
         <v>331</v>
       </c>
-      <c r="B479" s="14" t="s">
+      <c r="B479" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C479" s="14" t="str">
+      <c r="C479" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Text</v>
       </c>
@@ -20040,13 +20052,13 @@
       </c>
     </row>
     <row r="480" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A480" s="13" t="s">
+      <c r="A480" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B480" s="14" t="s">
+      <c r="B480" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C480" s="14" t="str">
+      <c r="C480" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Text</v>
       </c>
@@ -20061,13 +20073,13 @@
       </c>
     </row>
     <row r="481" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A481" s="13" t="s">
+      <c r="A481" s="12" t="s">
         <v>390</v>
       </c>
-      <c r="B481" s="14" t="s">
+      <c r="B481" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C481" s="14" t="str">
+      <c r="C481" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Lookup and reference</v>
       </c>
@@ -20082,13 +20094,13 @@
       </c>
     </row>
     <row r="482" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A482" s="13" t="s">
+      <c r="A482" s="12" t="s">
         <v>492</v>
       </c>
-      <c r="B482" s="14" t="s">
+      <c r="B482" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C482" s="14" t="str">
+      <c r="C482" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Look and reference</v>
       </c>
@@ -20103,13 +20115,13 @@
       </c>
     </row>
     <row r="483" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A483" s="13" t="s">
+      <c r="A483" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B483" s="14" t="s">
+      <c r="B483" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C483" s="14" t="str">
+      <c r="C483" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Lookup and reference</v>
       </c>
@@ -20124,13 +20136,13 @@
       </c>
     </row>
     <row r="484" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A484" s="13" t="s">
+      <c r="A484" s="12" t="s">
         <v>452</v>
       </c>
-      <c r="B484" s="14" t="s">
+      <c r="B484" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C484" s="14" t="str">
+      <c r="C484" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Date and time</v>
       </c>
@@ -20145,13 +20157,13 @@
       </c>
     </row>
     <row r="485" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A485" s="13" t="s">
+      <c r="A485" s="12" t="s">
         <v>453</v>
       </c>
-      <c r="B485" s="14" t="s">
+      <c r="B485" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C485" s="14" t="str">
+      <c r="C485" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Date and time</v>
       </c>
@@ -20166,13 +20178,13 @@
       </c>
     </row>
     <row r="486" spans="1:8" ht="63" x14ac:dyDescent="0.5">
-      <c r="A486" s="13" t="s">
+      <c r="A486" s="12" t="s">
         <v>378</v>
       </c>
-      <c r="B486" s="14" t="s">
+      <c r="B486" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C486" s="14" t="str">
+      <c r="C486" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Financial</v>
       </c>
@@ -20189,13 +20201,13 @@
       </c>
     </row>
     <row r="487" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A487" s="13" t="s">
+      <c r="A487" s="12" t="s">
         <v>249</v>
       </c>
-      <c r="B487" s="14" t="s">
+      <c r="B487" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C487" s="14" t="str">
+      <c r="C487" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Financial</v>
       </c>
@@ -20210,13 +20222,13 @@
       </c>
     </row>
     <row r="488" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A488" s="13" t="s">
+      <c r="A488" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="B488" s="14" t="s">
+      <c r="B488" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C488" s="14" t="str">
+      <c r="C488" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Financial</v>
       </c>
@@ -20231,13 +20243,13 @@
       </c>
     </row>
     <row r="489" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A489" s="13" t="s">
+      <c r="A489" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B489" s="14" t="s">
+      <c r="B489" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C489" s="14" t="str">
+      <c r="C489" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Financial</v>
       </c>
@@ -20252,13 +20264,13 @@
       </c>
     </row>
     <row r="490" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A490" s="13" t="s">
+      <c r="A490" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="B490" s="14" t="s">
+      <c r="B490" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C490" s="14" t="str">
+      <c r="C490" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Financial</v>
       </c>
@@ -20273,13 +20285,13 @@
       </c>
     </row>
     <row r="491" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A491" s="13" t="s">
+      <c r="A491" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="B491" s="14" t="s">
+      <c r="B491" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C491" s="14" t="str">
+      <c r="C491" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Financial</v>
       </c>
@@ -20294,13 +20306,13 @@
       </c>
     </row>
     <row r="492" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A492" s="13" t="s">
+      <c r="A492" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="B492" s="14" t="s">
+      <c r="B492" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C492" s="14" t="str">
+      <c r="C492" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Financial</v>
       </c>
@@ -20315,13 +20327,13 @@
       </c>
     </row>
     <row r="493" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A493" s="13" t="s">
+      <c r="A493" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B493" s="14" t="s">
+      <c r="B493" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C493" s="14" t="str">
+      <c r="C493" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Financial</v>
       </c>
@@ -20336,13 +20348,13 @@
       </c>
     </row>
     <row r="494" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A494" s="13" t="s">
+      <c r="A494" s="12" t="s">
         <v>250</v>
       </c>
-      <c r="B494" s="14" t="s">
+      <c r="B494" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C494" s="14" t="str">
+      <c r="C494" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Financial</v>
       </c>
@@ -20357,13 +20369,13 @@
       </c>
     </row>
     <row r="495" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A495" s="13" t="s">
+      <c r="A495" s="12" t="s">
         <v>391</v>
       </c>
-      <c r="B495" s="14" t="s">
+      <c r="B495" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C495" s="14" t="str">
+      <c r="C495" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Financial</v>
       </c>
@@ -20378,13 +20390,13 @@
       </c>
     </row>
     <row r="496" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A496" s="13" t="s">
+      <c r="A496" s="12" t="s">
         <v>504</v>
       </c>
-      <c r="B496" s="14" t="s">
+      <c r="B496" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C496" s="14" t="str">
+      <c r="C496" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Compatibility</v>
       </c>
@@ -20401,13 +20413,13 @@
       </c>
     </row>
     <row r="497" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
-      <c r="A497" s="13" t="s">
+      <c r="A497" s="12" t="s">
         <v>374</v>
       </c>
-      <c r="B497" s="14" t="s">
+      <c r="B497" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C497" s="14" t="str">
+      <c r="C497" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Math and trigonometry</v>
       </c>
@@ -20415,20 +20427,22 @@
         <v>994</v>
       </c>
       <c r="E497" s="8"/>
-      <c r="F497" s="8"/>
+      <c r="F497" s="8" t="s">
+        <v>1131</v>
+      </c>
       <c r="G497" s="8" t="s">
         <v>1091</v>
       </c>
       <c r="H497" s="8"/>
     </row>
     <row r="498" spans="1:8" ht="63" x14ac:dyDescent="0.5">
-      <c r="A498" s="13" t="s">
+      <c r="A498" s="12" t="s">
         <v>373</v>
       </c>
-      <c r="B498" s="14" t="s">
+      <c r="B498" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C498" s="14" t="str">
+      <c r="C498" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Math and trigonometry</v>
       </c>
@@ -20443,13 +20457,13 @@
       </c>
     </row>
     <row r="499" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
-      <c r="A499" s="13" t="s">
+      <c r="A499" s="12" t="s">
         <v>372</v>
       </c>
-      <c r="B499" s="14" t="s">
+      <c r="B499" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C499" s="14" t="str">
+      <c r="C499" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Math and trigonometry</v>
       </c>
@@ -20457,20 +20471,22 @@
         <v>996</v>
       </c>
       <c r="E499" s="8"/>
-      <c r="F499" s="8"/>
+      <c r="F499" s="8" t="s">
+        <v>1131</v>
+      </c>
       <c r="G499" s="8" t="s">
         <v>1091</v>
       </c>
       <c r="H499" s="8"/>
     </row>
     <row r="500" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A500" s="13" t="s">
+      <c r="A500" s="12" t="s">
         <v>457</v>
       </c>
-      <c r="B500" s="14" t="s">
+      <c r="B500" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C500" s="14" t="str">
+      <c r="C500" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Lookup and reference</v>
       </c>
@@ -20487,13 +20503,13 @@
       </c>
     </row>
     <row r="501" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A501" s="13" t="s">
+      <c r="A501" s="12" t="s">
         <v>458</v>
       </c>
-      <c r="B501" s="14" t="s">
+      <c r="B501" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C501" s="14" t="str">
+      <c r="C501" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Lookup and reference</v>
       </c>
@@ -20510,13 +20526,13 @@
       </c>
     </row>
     <row r="502" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A502" s="13" t="s">
+      <c r="A502" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="B502" s="14" t="s">
+      <c r="B502" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C502" s="14" t="str">
+      <c r="C502" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Financial</v>
       </c>
@@ -20531,13 +20547,13 @@
       </c>
     </row>
     <row r="503" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A503" s="13" t="s">
+      <c r="A503" s="12" t="s">
         <v>191</v>
       </c>
-      <c r="B503" s="14" t="s">
+      <c r="B503" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C503" s="14" t="str">
+      <c r="C503" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Financial</v>
       </c>
@@ -20552,13 +20568,13 @@
       </c>
     </row>
     <row r="504" spans="1:8" ht="63" x14ac:dyDescent="0.5">
-      <c r="A504" s="13" t="s">
+      <c r="A504" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="B504" s="14" t="s">
+      <c r="B504" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C504" s="14" t="str">
+      <c r="C504" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Math and trigonometry</v>
       </c>
@@ -20566,20 +20582,22 @@
         <v>1001</v>
       </c>
       <c r="E504" s="8"/>
-      <c r="F504" s="8"/>
+      <c r="F504" s="8" t="s">
+        <v>1131</v>
+      </c>
       <c r="G504" s="8" t="s">
         <v>1092</v>
       </c>
       <c r="H504" s="8"/>
     </row>
     <row r="505" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A505" s="13" t="s">
+      <c r="A505" s="12" t="s">
         <v>329</v>
       </c>
-      <c r="B505" s="14" t="s">
+      <c r="B505" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="C505" s="14" t="str">
+      <c r="C505" s="7" t="str">
         <f>_xlfn.TEXTBEFORE(Tabelle1[[#This Row],[Beschreibung]],":")</f>
         <v>Financial</v>
       </c>

</xml_diff>

<commit_message>
Gruppe A Funktionen zum Umsetzen ergänzt
</commit_message>
<xml_diff>
--- a/mgmt/Funktionsliste-Teamaufteilung.xlsx
+++ b/mgmt/Funktionsliste-Teamaufteilung.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hspforzheimde-my.sharepoint.com/personal/staibflo_hs-pforzheim_de/Documents/für HS/SE/GitHub/excelator/mgmt/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f68b39a81cc06860/Documents/GitHub/excelator/mgmt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{BD76375E-882C-934F-8082-3697347F1EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16C63939-05ED-4E9C-86A2-7B8FCBEAF6BC}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="13_ncr:1_{BD76375E-882C-934F-8082-3697347F1EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9392DDBD-FE83-4276-B583-565E5B85C598}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{1F02C744-EE90-A14B-9229-2ACDAC5D761E}"/>
+    <workbookView xWindow="-6375" yWindow="-12120" windowWidth="19440" windowHeight="11640" xr2:uid="{1F02C744-EE90-A14B-9229-2ACDAC5D761E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1989" uniqueCount="1133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2000" uniqueCount="1134">
   <si>
     <t>Funktionsname</t>
   </si>
@@ -9417,6 +9417,9 @@
   </si>
   <si>
     <t>&amp;</t>
+  </si>
+  <si>
+    <t>Wird umgesetzt</t>
   </si>
 </sst>
 </file>
@@ -9557,8 +9560,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
     <dxf>
@@ -9727,13 +9730,21 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C418F1F6-3AF5-EF4E-8CE1-8CA525105B91}" name="Tabelle1" displayName="Tabelle1" ref="A1:H505" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A1:H505" xr:uid="{C418F1F6-3AF5-EF4E-8CE1-8CA525105B91}"/>
+  <autoFilter ref="A1:H505" xr:uid="{C418F1F6-3AF5-EF4E-8CE1-8CA525105B91}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="A"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="6">
+      <filters>
+        <filter val="möglich"/>
+        <filter val="möglich aber unnötig ?"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H505">
     <sortCondition ref="A1:A505"/>
   </sortState>
@@ -9754,7 +9765,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -10052,22 +10063,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9E696CC-4DD8-8E43-8BCC-2210EBDA2D24}">
   <dimension ref="A1:J505"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A465" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.59765625" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="79.25" customWidth="1"/>
-    <col min="5" max="6" width="26.1875" customWidth="1"/>
-    <col min="7" max="7" width="17.8125" customWidth="1"/>
+    <col min="4" max="4" width="79.19921875" customWidth="1"/>
+    <col min="5" max="5" width="14.796875" customWidth="1"/>
+    <col min="6" max="6" width="14.19921875" customWidth="1"/>
+    <col min="7" max="7" width="17.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="64.2" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -10093,7 +10105,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="63" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:10" ht="78" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>387</v>
       </c>
@@ -10121,7 +10133,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:10" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -10144,7 +10156,7 @@
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:10" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
@@ -10167,7 +10179,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:10" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
@@ -10188,7 +10200,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:10" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
@@ -10209,7 +10221,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>11</v>
       </c>
@@ -10230,7 +10242,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>86</v>
       </c>
@@ -10251,7 +10263,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>87</v>
       </c>
@@ -10272,7 +10284,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>88</v>
       </c>
@@ -10293,7 +10305,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:10" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
@@ -10314,7 +10326,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:10" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>489</v>
       </c>
@@ -10335,7 +10347,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:10" ht="46.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>490</v>
       </c>
@@ -10356,7 +10368,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:10" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>4</v>
       </c>
@@ -10373,11 +10385,13 @@
       <c r="E14" s="8" t="s">
         <v>1017</v>
       </c>
-      <c r="F14" s="8"/>
+      <c r="F14" s="8" t="s">
+        <v>1077</v>
+      </c>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
     </row>
-    <row r="15" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:10" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>5</v>
       </c>
@@ -10394,11 +10408,13 @@
       <c r="E15" s="8" t="s">
         <v>1018</v>
       </c>
-      <c r="F15" s="8"/>
+      <c r="F15" s="8" t="s">
+        <v>1133</v>
+      </c>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
     </row>
-    <row r="16" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>6</v>
       </c>
@@ -10419,7 +10435,7 @@
       </c>
       <c r="H16" s="8"/>
     </row>
-    <row r="17" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>7</v>
       </c>
@@ -10440,7 +10456,7 @@
       </c>
       <c r="H17" s="8"/>
     </row>
-    <row r="18" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>17</v>
       </c>
@@ -10457,11 +10473,13 @@
       <c r="E18" s="8" t="s">
         <v>1021</v>
       </c>
-      <c r="F18" s="8"/>
+      <c r="F18" s="8" t="s">
+        <v>1133</v>
+      </c>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
     </row>
-    <row r="19" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>18</v>
       </c>
@@ -10478,11 +10496,13 @@
       <c r="E19" s="8" t="s">
         <v>1022</v>
       </c>
-      <c r="F19" s="8"/>
+      <c r="F19" s="8" t="s">
+        <v>1133</v>
+      </c>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
     </row>
-    <row r="20" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>19</v>
       </c>
@@ -10499,11 +10519,13 @@
       <c r="E20" s="8" t="s">
         <v>1023</v>
       </c>
-      <c r="F20" s="8"/>
+      <c r="F20" s="8" t="s">
+        <v>1133</v>
+      </c>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
     </row>
-    <row r="21" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>20</v>
       </c>
@@ -10524,7 +10546,7 @@
       </c>
       <c r="H21" s="8"/>
     </row>
-    <row r="22" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>21</v>
       </c>
@@ -10545,7 +10567,7 @@
       </c>
       <c r="H22" s="8"/>
     </row>
-    <row r="23" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>16</v>
       </c>
@@ -10566,7 +10588,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>2</v>
       </c>
@@ -10587,7 +10609,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>3</v>
       </c>
@@ -10608,7 +10630,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>51</v>
       </c>
@@ -10629,7 +10651,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="63" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:8" ht="78" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>388</v>
       </c>
@@ -10646,13 +10668,15 @@
       <c r="E27" s="8" t="s">
         <v>1025</v>
       </c>
-      <c r="F27" s="8"/>
+      <c r="F27" s="8" t="s">
+        <v>1133</v>
+      </c>
       <c r="G27" s="8" t="s">
         <v>1006</v>
       </c>
       <c r="H27" s="8"/>
     </row>
-    <row r="28" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>379</v>
       </c>
@@ -10673,7 +10697,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>27</v>
       </c>
@@ -10694,7 +10718,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
         <v>28</v>
       </c>
@@ -10715,7 +10739,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>14</v>
       </c>
@@ -10736,7 +10760,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>29</v>
       </c>
@@ -10757,7 +10781,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>30</v>
       </c>
@@ -10778,7 +10802,7 @@
       </c>
       <c r="H33" s="8"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
         <v>31</v>
       </c>
@@ -10799,7 +10823,7 @@
       </c>
       <c r="H34" s="8"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>32</v>
       </c>
@@ -10820,7 +10844,7 @@
       </c>
       <c r="H35" s="8"/>
     </row>
-    <row r="36" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
         <v>36</v>
       </c>
@@ -10841,7 +10865,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
         <v>34</v>
       </c>
@@ -10862,7 +10886,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
         <v>33</v>
       </c>
@@ -10883,7 +10907,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>35</v>
       </c>
@@ -10904,7 +10928,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>37</v>
       </c>
@@ -10919,13 +10943,15 @@
         <v>545</v>
       </c>
       <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
+      <c r="F40" s="8" t="s">
+        <v>1133</v>
+      </c>
       <c r="G40" s="8" t="s">
         <v>1020</v>
       </c>
       <c r="H40" s="8"/>
     </row>
-    <row r="41" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>38</v>
       </c>
@@ -10946,7 +10972,7 @@
       </c>
       <c r="H41" s="8"/>
     </row>
-    <row r="42" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
         <v>39</v>
       </c>
@@ -10967,7 +10993,7 @@
       </c>
       <c r="H42" s="8"/>
     </row>
-    <row r="43" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
         <v>43</v>
       </c>
@@ -10988,7 +11014,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
         <v>41</v>
       </c>
@@ -11009,7 +11035,7 @@
       <c r="G44" s="8"/>
       <c r="H44" s="8"/>
     </row>
-    <row r="45" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
         <v>42</v>
       </c>
@@ -11030,7 +11056,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
         <v>40</v>
       </c>
@@ -11051,7 +11077,7 @@
       <c r="G46" s="8"/>
       <c r="H46" s="8"/>
     </row>
-    <row r="47" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
         <v>45</v>
       </c>
@@ -11072,7 +11098,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
         <v>46</v>
       </c>
@@ -11093,7 +11119,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
         <v>47</v>
       </c>
@@ -11114,7 +11140,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>44</v>
       </c>
@@ -11135,7 +11161,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="s">
         <v>48</v>
       </c>
@@ -11156,7 +11182,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="s">
         <v>401</v>
       </c>
@@ -11177,7 +11203,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
         <v>402</v>
       </c>
@@ -11198,7 +11224,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
         <v>371</v>
       </c>
@@ -11213,13 +11239,15 @@
         <v>559</v>
       </c>
       <c r="E54" s="8"/>
-      <c r="F54" s="8"/>
+      <c r="F54" s="8" t="s">
+        <v>1133</v>
+      </c>
       <c r="G54" s="8" t="s">
         <v>1024</v>
       </c>
       <c r="H54" s="8"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
         <v>416</v>
       </c>
@@ -11240,7 +11268,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
         <v>499</v>
       </c>
@@ -11261,7 +11289,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="s">
         <v>366</v>
       </c>
@@ -11282,7 +11310,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
         <v>52</v>
       </c>
@@ -11303,7 +11331,7 @@
       </c>
       <c r="H58" s="8"/>
     </row>
-    <row r="59" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="s">
         <v>55</v>
       </c>
@@ -11324,7 +11352,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="s">
         <v>57</v>
       </c>
@@ -11345,7 +11373,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
         <v>58</v>
       </c>
@@ -11366,7 +11394,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="6" t="s">
         <v>62</v>
       </c>
@@ -11387,7 +11415,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
         <v>63</v>
       </c>
@@ -11408,7 +11436,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="6" t="s">
         <v>64</v>
       </c>
@@ -11429,7 +11457,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="6" t="s">
         <v>60</v>
       </c>
@@ -11450,7 +11478,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="6" t="s">
         <v>61</v>
       </c>
@@ -11471,7 +11499,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="6" t="s">
         <v>59</v>
       </c>
@@ -11492,7 +11520,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="6" t="s">
         <v>69</v>
       </c>
@@ -11513,7 +11541,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="6" t="s">
         <v>70</v>
       </c>
@@ -11534,7 +11562,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="78.75" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:8" ht="78" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="6" t="s">
         <v>81</v>
       </c>
@@ -11557,7 +11585,7 @@
       </c>
       <c r="H70" s="8"/>
     </row>
-    <row r="71" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
         <v>82</v>
       </c>
@@ -11574,11 +11602,13 @@
       <c r="E71" s="8" t="s">
         <v>1029</v>
       </c>
-      <c r="F71" s="8"/>
+      <c r="F71" s="8" t="s">
+        <v>1133</v>
+      </c>
       <c r="G71" s="8"/>
       <c r="H71" s="8"/>
     </row>
-    <row r="72" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A72" s="6" t="s">
         <v>101</v>
       </c>
@@ -11599,7 +11629,7 @@
       </c>
       <c r="H72" s="8"/>
     </row>
-    <row r="73" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A73" s="6" t="s">
         <v>102</v>
       </c>
@@ -11620,7 +11650,7 @@
       </c>
       <c r="H73" s="8"/>
     </row>
-    <row r="74" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="6" t="s">
         <v>83</v>
       </c>
@@ -11641,7 +11671,7 @@
       <c r="G74" s="8"/>
       <c r="H74" s="8"/>
     </row>
-    <row r="75" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" s="6" t="s">
         <v>84</v>
       </c>
@@ -11662,7 +11692,7 @@
       <c r="G75" s="8"/>
       <c r="H75" s="8"/>
     </row>
-    <row r="76" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A76" s="6" t="s">
         <v>85</v>
       </c>
@@ -11677,13 +11707,15 @@
         <v>580</v>
       </c>
       <c r="E76" s="8"/>
-      <c r="F76" s="8"/>
+      <c r="F76" s="8" t="s">
+        <v>1133</v>
+      </c>
       <c r="G76" s="8" t="s">
         <v>1024</v>
       </c>
       <c r="H76" s="8"/>
     </row>
-    <row r="77" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="6" t="s">
         <v>97</v>
       </c>
@@ -11704,7 +11736,7 @@
       <c r="G77" s="8"/>
       <c r="H77" s="8"/>
     </row>
-    <row r="78" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="6" t="s">
         <v>98</v>
       </c>
@@ -11725,7 +11757,7 @@
       <c r="G78" s="8"/>
       <c r="H78" s="8"/>
     </row>
-    <row r="79" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="6" t="s">
         <v>99</v>
       </c>
@@ -11746,7 +11778,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:8" ht="46.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="6" t="s">
         <v>100</v>
       </c>
@@ -11767,7 +11799,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="63" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:8" ht="78" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="6" t="s">
         <v>103</v>
       </c>
@@ -11788,7 +11820,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="6" t="s">
         <v>104</v>
       </c>
@@ -11809,7 +11841,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:8" ht="46.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="6" t="s">
         <v>105</v>
       </c>
@@ -11830,7 +11862,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="6" t="s">
         <v>108</v>
       </c>
@@ -11851,7 +11883,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:8" ht="46.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="6" t="s">
         <v>106</v>
       </c>
@@ -11872,7 +11904,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:8" ht="46.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="6" t="s">
         <v>107</v>
       </c>
@@ -11893,7 +11925,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" s="6" t="s">
         <v>109</v>
       </c>
@@ -11914,7 +11946,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A88" s="6" t="s">
         <v>113</v>
       </c>
@@ -11929,13 +11961,15 @@
         <v>592</v>
       </c>
       <c r="E88" s="8"/>
-      <c r="F88" s="8"/>
+      <c r="F88" s="8" t="s">
+        <v>1133</v>
+      </c>
       <c r="G88" s="8" t="s">
         <v>1024</v>
       </c>
       <c r="H88" s="8"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" s="6" t="s">
         <v>112</v>
       </c>
@@ -11956,7 +11990,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" s="6" t="s">
         <v>114</v>
       </c>
@@ -11977,7 +12011,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" s="6" t="s">
         <v>121</v>
       </c>
@@ -11998,7 +12032,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" s="6" t="s">
         <v>122</v>
       </c>
@@ -12019,7 +12053,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" s="6" t="s">
         <v>131</v>
       </c>
@@ -12040,7 +12074,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="94" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" s="6" t="s">
         <v>120</v>
       </c>
@@ -12061,7 +12095,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" s="6" t="s">
         <v>133</v>
       </c>
@@ -12082,7 +12116,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" s="6" t="s">
         <v>134</v>
       </c>
@@ -12103,7 +12137,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" s="6" t="s">
         <v>115</v>
       </c>
@@ -12124,7 +12158,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" s="6" t="s">
         <v>138</v>
       </c>
@@ -12145,7 +12179,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="99" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" s="6" t="s">
         <v>140</v>
       </c>
@@ -12166,7 +12200,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="100" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" s="6" t="s">
         <v>141</v>
       </c>
@@ -12187,7 +12221,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="101" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" s="6" t="s">
         <v>142</v>
       </c>
@@ -12208,7 +12242,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="102" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" s="6" t="s">
         <v>144</v>
       </c>
@@ -12227,7 +12261,7 @@
       <c r="G102" s="8"/>
       <c r="H102" s="8"/>
     </row>
-    <row r="103" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="103" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" s="6" t="s">
         <v>145</v>
       </c>
@@ -12246,7 +12280,7 @@
       <c r="G103" s="8"/>
       <c r="H103" s="8"/>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" s="6" t="s">
         <v>129</v>
       </c>
@@ -12265,7 +12299,7 @@
       <c r="G104" s="8"/>
       <c r="H104" s="8"/>
     </row>
-    <row r="105" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="105" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" s="6" t="s">
         <v>127</v>
       </c>
@@ -12284,7 +12318,7 @@
       <c r="G105" s="8"/>
       <c r="H105" s="8"/>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" s="6" t="s">
         <v>124</v>
       </c>
@@ -12303,7 +12337,7 @@
       <c r="G106" s="8"/>
       <c r="H106" s="8"/>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" s="6" t="s">
         <v>125</v>
       </c>
@@ -12322,7 +12356,7 @@
       <c r="G107" s="8"/>
       <c r="H107" s="8"/>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="108" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" s="6" t="s">
         <v>126</v>
       </c>
@@ -12341,7 +12375,7 @@
       <c r="G108" s="8"/>
       <c r="H108" s="8"/>
     </row>
-    <row r="109" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="109" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" s="6" t="s">
         <v>435</v>
       </c>
@@ -12360,7 +12394,7 @@
       <c r="G109" s="8"/>
       <c r="H109" s="8"/>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="110" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" s="6" t="s">
         <v>132</v>
       </c>
@@ -12379,7 +12413,7 @@
       <c r="G110" s="8"/>
       <c r="H110" s="8"/>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="111" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" s="6" t="s">
         <v>135</v>
       </c>
@@ -12398,7 +12432,7 @@
       <c r="G111" s="8"/>
       <c r="H111" s="8"/>
     </row>
-    <row r="112" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="112" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" s="6" t="s">
         <v>143</v>
       </c>
@@ -12417,7 +12451,7 @@
       <c r="G112" s="8"/>
       <c r="H112" s="8"/>
     </row>
-    <row r="113" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="113" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" s="6" t="s">
         <v>146</v>
       </c>
@@ -12436,7 +12470,7 @@
       <c r="G113" s="8"/>
       <c r="H113" s="8"/>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" s="6" t="s">
         <v>147</v>
       </c>
@@ -12455,7 +12489,7 @@
       <c r="G114" s="8"/>
       <c r="H114" s="8"/>
     </row>
-    <row r="115" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="115" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" s="6" t="s">
         <v>471</v>
       </c>
@@ -12474,7 +12508,7 @@
       <c r="G115" s="8"/>
       <c r="H115" s="8"/>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" s="6" t="s">
         <v>148</v>
       </c>
@@ -12493,7 +12527,7 @@
       <c r="G116" s="8"/>
       <c r="H116" s="8"/>
     </row>
-    <row r="117" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="117" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" s="6" t="s">
         <v>382</v>
       </c>
@@ -12512,7 +12546,7 @@
       <c r="G117" s="8"/>
       <c r="H117" s="8"/>
     </row>
-    <row r="118" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="118" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" s="6" t="s">
         <v>159</v>
       </c>
@@ -12531,7 +12565,7 @@
       <c r="G118" s="8"/>
       <c r="H118" s="8"/>
     </row>
-    <row r="119" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="119" spans="1:8" ht="62.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" s="6" t="s">
         <v>155</v>
       </c>
@@ -12550,7 +12584,7 @@
       <c r="G119" s="8"/>
       <c r="H119" s="8"/>
     </row>
-    <row r="120" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="120" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" s="6" t="s">
         <v>158</v>
       </c>
@@ -12569,7 +12603,7 @@
       <c r="G120" s="8"/>
       <c r="H120" s="8"/>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="6" t="s">
         <v>160</v>
       </c>
@@ -12588,7 +12622,7 @@
       <c r="G121" s="8"/>
       <c r="H121" s="8"/>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" s="6" t="s">
         <v>161</v>
       </c>
@@ -12607,7 +12641,7 @@
       <c r="G122" s="8"/>
       <c r="H122" s="8"/>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" s="6" t="s">
         <v>171</v>
       </c>
@@ -12626,7 +12660,7 @@
       <c r="G123" s="8"/>
       <c r="H123" s="8"/>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" s="6" t="s">
         <v>172</v>
       </c>
@@ -12645,7 +12679,7 @@
       <c r="G124" s="8"/>
       <c r="H124" s="8"/>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="125" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" s="6" t="s">
         <v>188</v>
       </c>
@@ -12664,7 +12698,7 @@
       <c r="G125" s="8"/>
       <c r="H125" s="8"/>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" s="6" t="s">
         <v>165</v>
       </c>
@@ -12683,7 +12717,7 @@
       <c r="G126" s="8"/>
       <c r="H126" s="8"/>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" s="6" t="s">
         <v>167</v>
       </c>
@@ -12702,7 +12736,7 @@
       <c r="G127" s="8"/>
       <c r="H127" s="8"/>
     </row>
-    <row r="128" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="128" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" s="6" t="s">
         <v>162</v>
       </c>
@@ -12721,7 +12755,7 @@
       <c r="G128" s="8"/>
       <c r="H128" s="8"/>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" s="6" t="s">
         <v>164</v>
       </c>
@@ -12740,7 +12774,7 @@
       <c r="G129" s="8"/>
       <c r="H129" s="8"/>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="130" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" s="6" t="s">
         <v>166</v>
       </c>
@@ -12759,7 +12793,7 @@
       <c r="G130" s="8"/>
       <c r="H130" s="8"/>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="131" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" s="6" t="s">
         <v>154</v>
       </c>
@@ -12778,7 +12812,7 @@
       <c r="G131" s="8"/>
       <c r="H131" s="8"/>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" s="6" t="s">
         <v>176</v>
       </c>
@@ -12797,7 +12831,7 @@
       <c r="G132" s="8"/>
       <c r="H132" s="8"/>
     </row>
-    <row r="133" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="133" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" s="6" t="s">
         <v>168</v>
       </c>
@@ -12816,7 +12850,7 @@
       <c r="G133" s="8"/>
       <c r="H133" s="8"/>
     </row>
-    <row r="134" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="134" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" s="6" t="s">
         <v>170</v>
       </c>
@@ -12835,7 +12869,7 @@
       <c r="G134" s="8"/>
       <c r="H134" s="8"/>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" s="6" t="s">
         <v>173</v>
       </c>
@@ -12854,7 +12888,7 @@
       <c r="G135" s="8"/>
       <c r="H135" s="8"/>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="136" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" s="6" t="s">
         <v>174</v>
       </c>
@@ -12873,7 +12907,7 @@
       <c r="G136" s="8"/>
       <c r="H136" s="8"/>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" s="6" t="s">
         <v>175</v>
       </c>
@@ -12892,7 +12926,7 @@
       <c r="G137" s="8"/>
       <c r="H137" s="8"/>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="138" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" s="6" t="s">
         <v>186</v>
       </c>
@@ -12911,7 +12945,7 @@
       <c r="G138" s="8"/>
       <c r="H138" s="8"/>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="139" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" s="6" t="s">
         <v>187</v>
       </c>
@@ -12930,7 +12964,7 @@
       <c r="G139" s="8"/>
       <c r="H139" s="8"/>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" s="6" t="s">
         <v>189</v>
       </c>
@@ -12949,7 +12983,7 @@
       <c r="G140" s="8"/>
       <c r="H140" s="8"/>
     </row>
-    <row r="141" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="141" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" s="6" t="s">
         <v>503</v>
       </c>
@@ -12968,7 +13002,7 @@
       <c r="G141" s="8"/>
       <c r="H141" s="8"/>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="142" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" s="6" t="s">
         <v>192</v>
       </c>
@@ -12987,7 +13021,7 @@
       <c r="G142" s="8"/>
       <c r="H142" s="8"/>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="143" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" s="6" t="s">
         <v>195</v>
       </c>
@@ -13006,7 +13040,7 @@
       <c r="G143" s="8"/>
       <c r="H143" s="8"/>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="144" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" s="6" t="s">
         <v>193</v>
       </c>
@@ -13025,7 +13059,7 @@
       <c r="G144" s="8"/>
       <c r="H144" s="8"/>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="145" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" s="6" t="s">
         <v>194</v>
       </c>
@@ -13044,7 +13078,7 @@
       <c r="G145" s="8"/>
       <c r="H145" s="8"/>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="146" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" s="6" t="s">
         <v>196</v>
       </c>
@@ -13063,7 +13097,7 @@
       <c r="G146" s="8"/>
       <c r="H146" s="8"/>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="147" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" s="6" t="s">
         <v>197</v>
       </c>
@@ -13082,7 +13116,7 @@
       <c r="G147" s="8"/>
       <c r="H147" s="8"/>
     </row>
-    <row r="148" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="148" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" s="6" t="s">
         <v>198</v>
       </c>
@@ -13101,7 +13135,7 @@
       <c r="G148" s="8"/>
       <c r="H148" s="8"/>
     </row>
-    <row r="149" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="149" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" s="6" t="s">
         <v>247</v>
       </c>
@@ -13120,7 +13154,7 @@
       <c r="G149" s="8"/>
       <c r="H149" s="8"/>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="150" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150" s="6" t="s">
         <v>199</v>
       </c>
@@ -13139,7 +13173,7 @@
       <c r="G150" s="8"/>
       <c r="H150" s="8"/>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="151" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" s="6" t="s">
         <v>150</v>
       </c>
@@ -13158,7 +13192,7 @@
       <c r="G151" s="8"/>
       <c r="H151" s="8"/>
     </row>
-    <row r="152" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="152" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" s="6" t="s">
         <v>151</v>
       </c>
@@ -13177,7 +13211,7 @@
       <c r="G152" s="8"/>
       <c r="H152" s="8"/>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="153" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" s="6" t="s">
         <v>152</v>
       </c>
@@ -13196,7 +13230,7 @@
       <c r="G153" s="8"/>
       <c r="H153" s="8"/>
     </row>
-    <row r="154" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="154" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" s="6" t="s">
         <v>153</v>
       </c>
@@ -13215,7 +13249,7 @@
       <c r="G154" s="8"/>
       <c r="H154" s="8"/>
     </row>
-    <row r="155" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="155" spans="1:8" ht="46.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" s="6" t="s">
         <v>123</v>
       </c>
@@ -13234,7 +13268,7 @@
       <c r="G155" s="8"/>
       <c r="H155" s="8"/>
     </row>
-    <row r="156" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="156" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" s="6" t="s">
         <v>119</v>
       </c>
@@ -13253,7 +13287,7 @@
       <c r="G156" s="8"/>
       <c r="H156" s="8"/>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="157" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" s="6" t="s">
         <v>201</v>
       </c>
@@ -13272,7 +13306,7 @@
       <c r="G157" s="8"/>
       <c r="H157" s="8"/>
     </row>
-    <row r="158" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="158" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" s="6" t="s">
         <v>156</v>
       </c>
@@ -13291,7 +13325,7 @@
       <c r="G158" s="8"/>
       <c r="H158" s="8"/>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="159" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" s="6" t="s">
         <v>463</v>
       </c>
@@ -13310,7 +13344,7 @@
       <c r="G159" s="8"/>
       <c r="H159" s="8"/>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="160" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" s="6" t="s">
         <v>202</v>
       </c>
@@ -13329,7 +13363,7 @@
       <c r="G160" s="8"/>
       <c r="H160" s="8"/>
     </row>
-    <row r="161" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="161" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161" s="6" t="s">
         <v>200</v>
       </c>
@@ -13348,7 +13382,7 @@
       <c r="G161" s="8"/>
       <c r="H161" s="8"/>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="162" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162" s="6" t="s">
         <v>462</v>
       </c>
@@ -13367,7 +13401,7 @@
       <c r="G162" s="8"/>
       <c r="H162" s="8"/>
     </row>
-    <row r="163" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="163" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" s="6" t="s">
         <v>128</v>
       </c>
@@ -13386,7 +13420,7 @@
       <c r="G163" s="8"/>
       <c r="H163" s="8"/>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="164" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164" s="6" t="s">
         <v>472</v>
       </c>
@@ -13405,7 +13439,7 @@
       <c r="G164" s="8"/>
       <c r="H164" s="8"/>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="165" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" s="6" t="s">
         <v>365</v>
       </c>
@@ -13424,7 +13458,7 @@
       <c r="G165" s="8"/>
       <c r="H165" s="8"/>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="166" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166" s="6" t="s">
         <v>204</v>
       </c>
@@ -13443,7 +13477,7 @@
       <c r="G166" s="8"/>
       <c r="H166" s="8"/>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="167" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167" s="6" t="s">
         <v>205</v>
       </c>
@@ -13462,7 +13496,7 @@
       <c r="G167" s="8"/>
       <c r="H167" s="8"/>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="168" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" s="6" t="s">
         <v>459</v>
       </c>
@@ -13481,7 +13515,7 @@
       <c r="G168" s="8"/>
       <c r="H168" s="8"/>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="169" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A169" s="6" t="s">
         <v>206</v>
       </c>
@@ -13500,7 +13534,7 @@
       <c r="G169" s="8"/>
       <c r="H169" s="8"/>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="170" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170" s="6" t="s">
         <v>207</v>
       </c>
@@ -13519,7 +13553,7 @@
       <c r="G170" s="8"/>
       <c r="H170" s="8"/>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="171" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" s="6" t="s">
         <v>208</v>
       </c>
@@ -13538,7 +13572,7 @@
       <c r="G171" s="8"/>
       <c r="H171" s="8"/>
     </row>
-    <row r="172" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="172" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" s="6" t="s">
         <v>211</v>
       </c>
@@ -13557,7 +13591,7 @@
       <c r="G172" s="8"/>
       <c r="H172" s="8"/>
     </row>
-    <row r="173" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="173" spans="1:8" ht="46.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" s="6" t="s">
         <v>212</v>
       </c>
@@ -13576,7 +13610,7 @@
       <c r="G173" s="8"/>
       <c r="H173" s="8"/>
     </row>
-    <row r="174" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="174" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" s="6" t="s">
         <v>213</v>
       </c>
@@ -13595,7 +13629,7 @@
       <c r="G174" s="8"/>
       <c r="H174" s="8"/>
     </row>
-    <row r="175" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="175" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175" s="6" t="s">
         <v>214</v>
       </c>
@@ -13614,7 +13648,7 @@
       <c r="G175" s="8"/>
       <c r="H175" s="8"/>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="176" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" s="6" t="s">
         <v>157</v>
       </c>
@@ -13633,7 +13667,7 @@
       <c r="G176" s="8"/>
       <c r="H176" s="8"/>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="177" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" s="6" t="s">
         <v>251</v>
       </c>
@@ -13652,7 +13686,7 @@
       <c r="G177" s="8"/>
       <c r="H177" s="8"/>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="178" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178" s="6" t="s">
         <v>219</v>
       </c>
@@ -13671,7 +13705,7 @@
       <c r="G178" s="8"/>
       <c r="H178" s="8"/>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="179" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179" s="6" t="s">
         <v>220</v>
       </c>
@@ -13690,7 +13724,7 @@
       <c r="G179" s="8"/>
       <c r="H179" s="8"/>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="180" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180" s="6" t="s">
         <v>233</v>
       </c>
@@ -13709,7 +13743,7 @@
       <c r="G180" s="8"/>
       <c r="H180" s="8"/>
     </row>
-    <row r="181" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="181" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181" s="6" t="s">
         <v>221</v>
       </c>
@@ -13728,7 +13762,7 @@
       <c r="G181" s="8"/>
       <c r="H181" s="8"/>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="182" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A182" s="6" t="s">
         <v>223</v>
       </c>
@@ -13747,7 +13781,7 @@
       <c r="G182" s="8"/>
       <c r="H182" s="8"/>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="183" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A183" s="6" t="s">
         <v>226</v>
       </c>
@@ -13766,7 +13800,7 @@
       <c r="G183" s="8"/>
       <c r="H183" s="8"/>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="184" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A184" s="6" t="s">
         <v>227</v>
       </c>
@@ -13785,7 +13819,7 @@
       <c r="G184" s="8"/>
       <c r="H184" s="8"/>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="185" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A185" s="6" t="s">
         <v>224</v>
       </c>
@@ -13804,7 +13838,7 @@
       <c r="G185" s="8"/>
       <c r="H185" s="8"/>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="186" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A186" s="6" t="s">
         <v>225</v>
       </c>
@@ -13823,7 +13857,7 @@
       <c r="G186" s="8"/>
       <c r="H186" s="8"/>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="187" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A187" s="6" t="s">
         <v>228</v>
       </c>
@@ -13842,7 +13876,7 @@
       <c r="G187" s="8"/>
       <c r="H187" s="8"/>
     </row>
-    <row r="188" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="188" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A188" s="6" t="s">
         <v>229</v>
       </c>
@@ -13861,7 +13895,7 @@
       <c r="G188" s="8"/>
       <c r="H188" s="8"/>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A189" s="6" t="s">
         <v>222</v>
       </c>
@@ -13880,7 +13914,7 @@
       <c r="G189" s="8"/>
       <c r="H189" s="8"/>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A190" s="6" t="s">
         <v>230</v>
       </c>
@@ -13899,7 +13933,7 @@
       <c r="G190" s="8"/>
       <c r="H190" s="8"/>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A191" s="6" t="s">
         <v>231</v>
       </c>
@@ -13918,7 +13952,7 @@
       <c r="G191" s="8"/>
       <c r="H191" s="8"/>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="192" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A192" s="6" t="s">
         <v>232</v>
       </c>
@@ -13937,7 +13971,7 @@
       <c r="G192" s="8"/>
       <c r="H192" s="8"/>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="193" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A193" s="6" t="s">
         <v>234</v>
       </c>
@@ -13956,7 +13990,7 @@
       <c r="G193" s="8"/>
       <c r="H193" s="8"/>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="194" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A194" s="6" t="s">
         <v>235</v>
       </c>
@@ -13975,7 +14009,7 @@
       <c r="G194" s="8"/>
       <c r="H194" s="8"/>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="195" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A195" s="6" t="s">
         <v>236</v>
       </c>
@@ -13994,7 +14028,7 @@
       <c r="G195" s="8"/>
       <c r="H195" s="8"/>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="196" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A196" s="6" t="s">
         <v>237</v>
       </c>
@@ -14013,7 +14047,7 @@
       <c r="G196" s="8"/>
       <c r="H196" s="8"/>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="197" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197" s="6" t="s">
         <v>238</v>
       </c>
@@ -14032,7 +14066,7 @@
       <c r="G197" s="8"/>
       <c r="H197" s="8"/>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="198" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A198" s="6" t="s">
         <v>239</v>
       </c>
@@ -14051,7 +14085,7 @@
       <c r="G198" s="8"/>
       <c r="H198" s="8"/>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="199" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A199" s="6" t="s">
         <v>241</v>
       </c>
@@ -14070,7 +14104,7 @@
       <c r="G199" s="8"/>
       <c r="H199" s="8"/>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="200" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A200" s="6" t="s">
         <v>242</v>
       </c>
@@ -14089,7 +14123,7 @@
       <c r="G200" s="8"/>
       <c r="H200" s="8"/>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="201" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A201" s="6" t="s">
         <v>243</v>
       </c>
@@ -14108,7 +14142,7 @@
       <c r="G201" s="8"/>
       <c r="H201" s="8"/>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="202" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A202" s="6" t="s">
         <v>240</v>
       </c>
@@ -14127,7 +14161,7 @@
       <c r="G202" s="8"/>
       <c r="H202" s="8"/>
     </row>
-    <row r="203" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="203" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203" s="6" t="s">
         <v>244</v>
       </c>
@@ -14146,7 +14180,7 @@
       <c r="G203" s="8"/>
       <c r="H203" s="8"/>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="204" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204" s="6" t="s">
         <v>245</v>
       </c>
@@ -14165,7 +14199,7 @@
       <c r="G204" s="8"/>
       <c r="H204" s="8"/>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="205" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A205" s="6" t="s">
         <v>246</v>
       </c>
@@ -14186,7 +14220,7 @@
       </c>
       <c r="H205" s="8"/>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="206" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A206" s="6" t="s">
         <v>248</v>
       </c>
@@ -14209,7 +14243,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="207" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="207" spans="1:8" ht="46.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A207" s="6" t="s">
         <v>265</v>
       </c>
@@ -14230,7 +14264,7 @@
       </c>
       <c r="H207" s="8"/>
     </row>
-    <row r="208" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="208" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A208" s="6" t="s">
         <v>266</v>
       </c>
@@ -14251,7 +14285,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="209" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="209" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A209" s="6" t="s">
         <v>267</v>
       </c>
@@ -14274,7 +14308,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="210" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A210" s="6" t="s">
         <v>263</v>
       </c>
@@ -14295,7 +14329,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="211" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A211" s="6" t="s">
         <v>253</v>
       </c>
@@ -14316,7 +14350,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="212" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A212" s="6" t="s">
         <v>254</v>
       </c>
@@ -14337,7 +14371,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="213" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="213" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A213" s="6" t="s">
         <v>256</v>
       </c>
@@ -14358,7 +14392,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="214" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A214" s="6" t="s">
         <v>255</v>
       </c>
@@ -14379,7 +14413,7 @@
       </c>
       <c r="H214" s="8"/>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="215" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A215" s="6" t="s">
         <v>259</v>
       </c>
@@ -14400,7 +14434,7 @@
       </c>
       <c r="H215" s="8"/>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="216" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A216" s="6" t="s">
         <v>252</v>
       </c>
@@ -14421,7 +14455,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="217" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A217" s="6" t="s">
         <v>257</v>
       </c>
@@ -14442,7 +14476,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="218" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A218" s="6" t="s">
         <v>258</v>
       </c>
@@ -14463,7 +14497,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="219" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A219" s="6" t="s">
         <v>264</v>
       </c>
@@ -14484,7 +14518,7 @@
       </c>
       <c r="H219" s="8"/>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="220" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A220" s="6" t="s">
         <v>261</v>
       </c>
@@ -14505,7 +14539,7 @@
       </c>
       <c r="H220" s="8"/>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="221" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A221" s="6" t="s">
         <v>260</v>
       </c>
@@ -14526,7 +14560,7 @@
       </c>
       <c r="H221" s="8"/>
     </row>
-    <row r="222" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="222" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A222" s="6" t="s">
         <v>498</v>
       </c>
@@ -14547,7 +14581,7 @@
       </c>
       <c r="H222" s="8"/>
     </row>
-    <row r="223" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="223" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A223" s="6" t="s">
         <v>328</v>
       </c>
@@ -14568,7 +14602,7 @@
       </c>
       <c r="H223" s="8"/>
     </row>
-    <row r="224" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="224" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A224" s="6" t="s">
         <v>268</v>
       </c>
@@ -14589,7 +14623,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="225" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="225" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A225" s="6" t="s">
         <v>486</v>
       </c>
@@ -14610,7 +14644,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="226" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="226" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A226" s="6" t="s">
         <v>359</v>
       </c>
@@ -14631,7 +14665,7 @@
       </c>
       <c r="H226" s="8"/>
     </row>
-    <row r="227" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="227" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A227" s="6" t="s">
         <v>271</v>
       </c>
@@ -14654,7 +14688,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="228" spans="1:8" ht="33" x14ac:dyDescent="0.7">
+    <row r="228" spans="1:8" ht="33" hidden="1" x14ac:dyDescent="0.45">
       <c r="A228" s="6" t="s">
         <v>272</v>
       </c>
@@ -14675,7 +14709,7 @@
       <c r="G228" s="8"/>
       <c r="H228" s="8"/>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="229" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A229" s="6" t="s">
         <v>410</v>
       </c>
@@ -14696,7 +14730,7 @@
       </c>
       <c r="H229" s="8"/>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="230" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A230" s="6" t="s">
         <v>286</v>
       </c>
@@ -14717,7 +14751,7 @@
       </c>
       <c r="H230" s="8"/>
     </row>
-    <row r="231" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="231" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A231" s="6" t="s">
         <v>72</v>
       </c>
@@ -14738,7 +14772,7 @@
       </c>
       <c r="H231" s="8"/>
     </row>
-    <row r="232" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="232" spans="1:8" ht="46.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A232" s="6" t="s">
         <v>73</v>
       </c>
@@ -14759,7 +14793,7 @@
       </c>
       <c r="H232" s="8"/>
     </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="233" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A233" s="6" t="s">
         <v>74</v>
       </c>
@@ -14780,7 +14814,7 @@
       </c>
       <c r="H233" s="8"/>
     </row>
-    <row r="234" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="234" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A234" s="6" t="s">
         <v>77</v>
       </c>
@@ -14803,7 +14837,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="235" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="235" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A235" s="6" t="s">
         <v>78</v>
       </c>
@@ -14826,7 +14860,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="236" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="236" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A236" s="6" t="s">
         <v>79</v>
       </c>
@@ -14849,7 +14883,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="237" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="237" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A237" s="6" t="s">
         <v>111</v>
       </c>
@@ -14872,7 +14906,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="238" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A238" s="6" t="s">
         <v>110</v>
       </c>
@@ -14895,7 +14929,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="239" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="239" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A239" s="6" t="s">
         <v>360</v>
       </c>
@@ -14918,7 +14952,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="240" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A240" s="6" t="s">
         <v>361</v>
       </c>
@@ -14941,7 +14975,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="241" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="241" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A241" s="6" t="s">
         <v>362</v>
       </c>
@@ -14964,7 +14998,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="242" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="242" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A242" s="6" t="s">
         <v>269</v>
       </c>
@@ -14985,7 +15019,7 @@
       </c>
       <c r="H242" s="8"/>
     </row>
-    <row r="243" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="243" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A243" s="6" t="s">
         <v>465</v>
       </c>
@@ -15006,7 +15040,7 @@
       </c>
       <c r="H243" s="8"/>
     </row>
-    <row r="244" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="244" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A244" s="6" t="s">
         <v>270</v>
       </c>
@@ -15027,7 +15061,7 @@
       </c>
       <c r="H244" s="8"/>
     </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="245" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A245" s="6" t="s">
         <v>274</v>
       </c>
@@ -15048,7 +15082,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="246" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="246" spans="1:8" ht="46.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A246" s="6" t="s">
         <v>275</v>
       </c>
@@ -15069,7 +15103,7 @@
       </c>
       <c r="H246" s="8"/>
     </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="247" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A247" s="6" t="s">
         <v>408</v>
       </c>
@@ -15092,7 +15126,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="248" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="248" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A248" s="6" t="s">
         <v>273</v>
       </c>
@@ -15113,7 +15147,7 @@
       </c>
       <c r="H248" s="8"/>
     </row>
-    <row r="249" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="249" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A249" s="6" t="s">
         <v>277</v>
       </c>
@@ -15134,7 +15168,7 @@
       <c r="G249" s="8"/>
       <c r="H249" s="8"/>
     </row>
-    <row r="250" spans="1:8" ht="33" x14ac:dyDescent="0.7">
+    <row r="250" spans="1:8" ht="33" hidden="1" x14ac:dyDescent="0.45">
       <c r="A250" s="6" t="s">
         <v>278</v>
       </c>
@@ -15155,7 +15189,7 @@
       <c r="G250" s="8"/>
       <c r="H250" s="8"/>
     </row>
-    <row r="251" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="251" spans="1:8" ht="46.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A251" s="6" t="s">
         <v>279</v>
       </c>
@@ -15176,7 +15210,7 @@
       <c r="G251" s="8"/>
       <c r="H251" s="8"/>
     </row>
-    <row r="252" spans="1:8" ht="409.5" x14ac:dyDescent="0.5">
+    <row r="252" spans="1:8" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A252" s="6" t="s">
         <v>280</v>
       </c>
@@ -15199,7 +15233,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="253" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A253" s="6" t="s">
         <v>281</v>
       </c>
@@ -15222,7 +15256,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="254" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A254" s="6" t="s">
         <v>284</v>
       </c>
@@ -15243,7 +15277,7 @@
       </c>
       <c r="H254" s="8"/>
     </row>
-    <row r="255" spans="1:8" ht="409.5" x14ac:dyDescent="0.5">
+    <row r="255" spans="1:8" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A255" s="6" t="s">
         <v>282</v>
       </c>
@@ -15266,7 +15300,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="256" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="256" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A256" s="6" t="s">
         <v>283</v>
       </c>
@@ -15287,7 +15321,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="257" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="257" spans="1:8" ht="46.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A257" s="6" t="s">
         <v>288</v>
       </c>
@@ -15308,7 +15342,7 @@
       </c>
       <c r="H257" s="8"/>
     </row>
-    <row r="258" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="258" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A258" s="6" t="s">
         <v>287</v>
       </c>
@@ -15331,7 +15365,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="259" spans="1:8" ht="63" x14ac:dyDescent="0.5">
+    <row r="259" spans="1:8" ht="62.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A259" s="6" t="s">
         <v>15</v>
       </c>
@@ -15354,7 +15388,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="260" spans="1:8" ht="18.75" x14ac:dyDescent="0.7">
+    <row r="260" spans="1:8" ht="19.2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A260" s="6" t="s">
         <v>290</v>
       </c>
@@ -15375,7 +15409,7 @@
       <c r="G260" s="8"/>
       <c r="H260" s="8"/>
     </row>
-    <row r="261" spans="1:8" ht="78.75" x14ac:dyDescent="0.5">
+    <row r="261" spans="1:8" ht="78" hidden="1" x14ac:dyDescent="0.3">
       <c r="A261" s="6" t="s">
         <v>291</v>
       </c>
@@ -15398,7 +15432,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="262" spans="1:8" ht="31.9" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="262" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A262" s="6" t="s">
         <v>292</v>
       </c>
@@ -15419,7 +15453,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="263" spans="1:8" ht="56.25" x14ac:dyDescent="0.7">
+    <row r="263" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A263" s="6" t="s">
         <v>293</v>
       </c>
@@ -15442,7 +15476,7 @@
       </c>
       <c r="H263" s="8"/>
     </row>
-    <row r="264" spans="1:8" ht="173.65" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="264" spans="1:8" ht="171.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A264" s="6" t="s">
         <v>294</v>
       </c>
@@ -15463,7 +15497,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="265" spans="1:8" ht="18.75" x14ac:dyDescent="0.5">
+    <row r="265" spans="1:8" ht="19.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A265" s="6" t="s">
         <v>295</v>
       </c>
@@ -15484,7 +15518,7 @@
       <c r="G265" s="8"/>
       <c r="H265" s="8"/>
     </row>
-    <row r="266" spans="1:8" ht="112.15" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="266" spans="1:8" ht="111" hidden="1" x14ac:dyDescent="0.45">
       <c r="A266" s="6" t="s">
         <v>311</v>
       </c>
@@ -15509,7 +15543,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="267" spans="1:8" ht="63" x14ac:dyDescent="0.5">
+    <row r="267" spans="1:8" ht="62.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A267" s="6" t="s">
         <v>297</v>
       </c>
@@ -15534,7 +15568,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="268" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="268" spans="1:8" ht="62.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A268" s="6" t="s">
         <v>299</v>
       </c>
@@ -15555,7 +15589,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="269" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="269" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A269" s="6" t="s">
         <v>300</v>
       </c>
@@ -15576,7 +15610,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="270" spans="1:8" ht="56.25" x14ac:dyDescent="0.5">
+    <row r="270" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A270" s="6" t="s">
         <v>301</v>
       </c>
@@ -15599,7 +15633,7 @@
       </c>
       <c r="H270" s="8"/>
     </row>
-    <row r="271" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="271" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A271" s="6" t="s">
         <v>298</v>
       </c>
@@ -15620,7 +15654,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="272" spans="1:8" ht="78.75" x14ac:dyDescent="0.5">
+    <row r="272" spans="1:8" ht="78" hidden="1" x14ac:dyDescent="0.3">
       <c r="A272" s="6" t="s">
         <v>22</v>
       </c>
@@ -15641,7 +15675,7 @@
       </c>
       <c r="H272" s="8"/>
     </row>
-    <row r="273" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="273" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A273" s="6" t="s">
         <v>23</v>
       </c>
@@ -15662,7 +15696,7 @@
       </c>
       <c r="H273" s="8"/>
     </row>
-    <row r="274" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="274" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A274" s="6" t="s">
         <v>24</v>
       </c>
@@ -15683,7 +15717,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="275" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="275" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A275" s="6" t="s">
         <v>25</v>
       </c>
@@ -15704,7 +15738,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="276" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="276" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A276" s="6" t="s">
         <v>26</v>
       </c>
@@ -15725,7 +15759,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="277" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="277" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A277" s="6" t="s">
         <v>303</v>
       </c>
@@ -15746,7 +15780,7 @@
       </c>
       <c r="H277" s="8"/>
     </row>
-    <row r="278" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="278" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A278" s="6" t="s">
         <v>305</v>
       </c>
@@ -15767,7 +15801,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="279" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="279" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A279" s="6" t="s">
         <v>306</v>
       </c>
@@ -15788,7 +15822,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="280" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="280" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A280" s="6" t="s">
         <v>307</v>
       </c>
@@ -15809,7 +15843,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="281" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="281" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A281" s="6" t="s">
         <v>308</v>
       </c>
@@ -15830,7 +15864,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="282" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="282" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A282" s="6" t="s">
         <v>149</v>
       </c>
@@ -15851,7 +15885,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="283" spans="1:8" ht="63" x14ac:dyDescent="0.5">
+    <row r="283" spans="1:8" ht="62.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A283" s="6" t="s">
         <v>460</v>
       </c>
@@ -15872,7 +15906,7 @@
       </c>
       <c r="H283" s="8"/>
     </row>
-    <row r="284" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="284" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A284" s="6" t="s">
         <v>312</v>
       </c>
@@ -15893,7 +15927,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="285" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="285" spans="1:8" ht="46.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A285" s="6" t="s">
         <v>49</v>
       </c>
@@ -15916,7 +15950,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="286" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="286" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A286" s="6" t="s">
         <v>50</v>
       </c>
@@ -15937,7 +15971,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="287" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="287" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A287" s="6" t="s">
         <v>330</v>
       </c>
@@ -15960,7 +15994,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="288" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="288" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A288" s="6" t="s">
         <v>314</v>
       </c>
@@ -15981,7 +16015,7 @@
       </c>
       <c r="H288" s="8"/>
     </row>
-    <row r="289" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="289" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A289" s="6" t="s">
         <v>315</v>
       </c>
@@ -16002,7 +16036,7 @@
       </c>
       <c r="H289" s="8"/>
     </row>
-    <row r="290" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="290" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A290" s="6" t="s">
         <v>316</v>
       </c>
@@ -16025,7 +16059,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="291" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="291" spans="1:8" ht="46.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A291" s="6" t="s">
         <v>317</v>
       </c>
@@ -16046,7 +16080,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="292" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="292" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A292" s="6" t="s">
         <v>327</v>
       </c>
@@ -16069,7 +16103,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="293" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="293" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A293" s="6" t="s">
         <v>318</v>
       </c>
@@ -16090,7 +16124,7 @@
       </c>
       <c r="H293" s="8"/>
     </row>
-    <row r="294" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="294" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A294" s="6" t="s">
         <v>322</v>
       </c>
@@ -16113,7 +16147,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="295" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="295" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A295" s="6" t="s">
         <v>325</v>
       </c>
@@ -16134,7 +16168,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="296" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="296" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A296" s="6" t="s">
         <v>323</v>
       </c>
@@ -16155,7 +16189,7 @@
       </c>
       <c r="H296" s="8"/>
     </row>
-    <row r="297" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="297" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A297" s="6" t="s">
         <v>319</v>
       </c>
@@ -16176,7 +16210,7 @@
       </c>
       <c r="H297" s="8"/>
     </row>
-    <row r="298" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="298" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A298" s="6" t="s">
         <v>320</v>
       </c>
@@ -16197,7 +16231,7 @@
       </c>
       <c r="H298" s="8"/>
     </row>
-    <row r="299" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="299" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A299" s="6" t="s">
         <v>321</v>
       </c>
@@ -16220,7 +16254,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="300" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="300" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A300" s="6" t="s">
         <v>324</v>
       </c>
@@ -16239,7 +16273,7 @@
       <c r="G300" s="8"/>
       <c r="H300" s="8"/>
     </row>
-    <row r="301" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="301" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A301" s="6" t="s">
         <v>326</v>
       </c>
@@ -16258,7 +16292,7 @@
       <c r="G301" s="8"/>
       <c r="H301" s="8"/>
     </row>
-    <row r="302" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="302" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A302" s="6" t="s">
         <v>137</v>
       </c>
@@ -16277,7 +16311,7 @@
       <c r="G302" s="8"/>
       <c r="H302" s="8"/>
     </row>
-    <row r="303" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="303" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A303" s="6" t="s">
         <v>136</v>
       </c>
@@ -16296,7 +16330,7 @@
       <c r="G303" s="8"/>
       <c r="H303" s="8"/>
     </row>
-    <row r="304" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="304" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A304" s="6" t="s">
         <v>313</v>
       </c>
@@ -16315,7 +16349,7 @@
       <c r="G304" s="8"/>
       <c r="H304" s="8"/>
     </row>
-    <row r="305" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="305" spans="1:8" ht="46.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A305" s="6" t="s">
         <v>54</v>
       </c>
@@ -16334,7 +16368,7 @@
       <c r="G305" s="8"/>
       <c r="H305" s="8"/>
     </row>
-    <row r="306" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="306" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A306" s="6" t="s">
         <v>53</v>
       </c>
@@ -16353,7 +16387,7 @@
       <c r="G306" s="8"/>
       <c r="H306" s="8"/>
     </row>
-    <row r="307" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="307" spans="1:8" ht="46.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A307" s="6" t="s">
         <v>341</v>
       </c>
@@ -16376,7 +16410,7 @@
       </c>
       <c r="H307" s="8"/>
     </row>
-    <row r="308" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="308" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A308" s="6" t="s">
         <v>340</v>
       </c>
@@ -16399,7 +16433,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="309" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="309" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A309" s="6" t="s">
         <v>332</v>
       </c>
@@ -16420,7 +16454,7 @@
       </c>
       <c r="H309" s="8"/>
     </row>
-    <row r="310" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="310" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A310" s="6" t="s">
         <v>333</v>
       </c>
@@ -16441,7 +16475,7 @@
       </c>
       <c r="H310" s="8"/>
     </row>
-    <row r="311" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="311" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A311" s="6" t="s">
         <v>334</v>
       </c>
@@ -16462,7 +16496,7 @@
       </c>
       <c r="H311" s="8"/>
     </row>
-    <row r="312" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="312" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A312" s="6" t="s">
         <v>342</v>
       </c>
@@ -16483,7 +16517,7 @@
       </c>
       <c r="H312" s="8"/>
     </row>
-    <row r="313" spans="1:8" ht="78.75" x14ac:dyDescent="0.5">
+    <row r="313" spans="1:8" ht="78" hidden="1" x14ac:dyDescent="0.3">
       <c r="A313" s="6" t="s">
         <v>343</v>
       </c>
@@ -16506,7 +16540,7 @@
       </c>
       <c r="H313" s="8"/>
     </row>
-    <row r="314" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="314" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A314" s="6" t="s">
         <v>346</v>
       </c>
@@ -16525,7 +16559,7 @@
       <c r="G314" s="8"/>
       <c r="H314" s="8"/>
     </row>
-    <row r="315" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="315" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A315" s="6" t="s">
         <v>349</v>
       </c>
@@ -16548,7 +16582,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="316" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="316" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A316" s="6" t="s">
         <v>352</v>
       </c>
@@ -16571,7 +16605,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="317" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="317" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A317" s="6" t="s">
         <v>353</v>
       </c>
@@ -16594,7 +16628,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="318" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="318" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A318" s="6" t="s">
         <v>354</v>
       </c>
@@ -16617,7 +16651,7 @@
       </c>
       <c r="H318" s="8"/>
     </row>
-    <row r="319" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="319" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A319" s="6" t="s">
         <v>203</v>
       </c>
@@ -16640,7 +16674,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="320" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="320" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A320" s="6" t="s">
         <v>357</v>
       </c>
@@ -16661,7 +16695,7 @@
       </c>
       <c r="H320" s="8"/>
     </row>
-    <row r="321" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="321" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A321" s="6" t="s">
         <v>356</v>
       </c>
@@ -16682,7 +16716,7 @@
       </c>
       <c r="H321" s="8"/>
     </row>
-    <row r="322" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="322" spans="1:8" ht="46.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A322" s="6" t="s">
         <v>310</v>
       </c>
@@ -16705,7 +16739,7 @@
       </c>
       <c r="H322" s="8"/>
     </row>
-    <row r="323" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="323" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A323" s="6" t="s">
         <v>358</v>
       </c>
@@ -16726,7 +16760,7 @@
       </c>
       <c r="H323" s="8"/>
     </row>
-    <row r="324" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="324" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A324" s="6" t="s">
         <v>400</v>
       </c>
@@ -16747,7 +16781,7 @@
       </c>
       <c r="H324" s="8"/>
     </row>
-    <row r="325" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="325" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A325" s="6" t="s">
         <v>364</v>
       </c>
@@ -16768,7 +16802,7 @@
       </c>
       <c r="H325" s="8"/>
     </row>
-    <row r="326" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="326" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A326" s="6" t="s">
         <v>181</v>
       </c>
@@ -16789,7 +16823,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="327" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="327" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A327" s="6" t="s">
         <v>182</v>
       </c>
@@ -16810,7 +16844,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="328" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="328" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A328" s="6" t="s">
         <v>183</v>
       </c>
@@ -16831,7 +16865,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="329" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="329" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A329" s="6" t="s">
         <v>184</v>
       </c>
@@ -16852,7 +16886,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="330" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="330" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A330" s="6" t="s">
         <v>185</v>
       </c>
@@ -16873,7 +16907,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="331" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="331" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A331" s="6" t="s">
         <v>302</v>
       </c>
@@ -16894,7 +16928,7 @@
       </c>
       <c r="H331" s="8"/>
     </row>
-    <row r="332" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="332" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A332" s="6" t="s">
         <v>430</v>
       </c>
@@ -16915,7 +16949,7 @@
       </c>
       <c r="H332" s="8"/>
     </row>
-    <row r="333" spans="1:8" ht="157.5" x14ac:dyDescent="0.5">
+    <row r="333" spans="1:8" ht="156" hidden="1" x14ac:dyDescent="0.3">
       <c r="A333" s="6" t="s">
         <v>344</v>
       </c>
@@ -16938,7 +16972,7 @@
       </c>
       <c r="H333" s="8"/>
     </row>
-    <row r="334" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="334" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A334" s="6" t="s">
         <v>345</v>
       </c>
@@ -16959,7 +16993,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="335" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="335" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A335" s="6" t="s">
         <v>347</v>
       </c>
@@ -16980,7 +17014,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="336" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="336" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A336" s="6" t="s">
         <v>348</v>
       </c>
@@ -17001,7 +17035,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="337" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="337" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A337" s="6" t="s">
         <v>367</v>
       </c>
@@ -17022,7 +17056,7 @@
         <v>1109</v>
       </c>
     </row>
-    <row r="338" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="338" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A338" s="6" t="s">
         <v>368</v>
       </c>
@@ -17043,7 +17077,7 @@
         <v>1109</v>
       </c>
     </row>
-    <row r="339" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="339" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A339" s="6" t="s">
         <v>369</v>
       </c>
@@ -17064,7 +17098,7 @@
         <v>1109</v>
       </c>
     </row>
-    <row r="340" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="340" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A340" s="6" t="s">
         <v>370</v>
       </c>
@@ -17085,7 +17119,7 @@
       </c>
       <c r="H340" s="8"/>
     </row>
-    <row r="341" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="341" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A341" s="6" t="s">
         <v>376</v>
       </c>
@@ -17106,7 +17140,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="342" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="342" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A342" s="6" t="s">
         <v>375</v>
       </c>
@@ -17127,7 +17161,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="343" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="343" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A343" s="6" t="s">
         <v>377</v>
       </c>
@@ -17148,7 +17182,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="344" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="344" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A344" s="6" t="s">
         <v>384</v>
       </c>
@@ -17171,7 +17205,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="345" spans="1:8" ht="63" x14ac:dyDescent="0.5">
+    <row r="345" spans="1:8" ht="62.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A345" s="6" t="s">
         <v>380</v>
       </c>
@@ -17194,7 +17228,7 @@
       </c>
       <c r="H345" s="8"/>
     </row>
-    <row r="346" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="346" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A346" s="6" t="s">
         <v>381</v>
       </c>
@@ -17215,7 +17249,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="347" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="347" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A347" s="6" t="s">
         <v>500</v>
       </c>
@@ -17236,7 +17270,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="348" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="348" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A348" s="6" t="s">
         <v>501</v>
       </c>
@@ -17257,7 +17291,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="349" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="349" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A349" s="6" t="s">
         <v>502</v>
       </c>
@@ -17278,7 +17312,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="350" spans="1:8" ht="63" x14ac:dyDescent="0.5">
+    <row r="350" spans="1:8" ht="62.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A350" s="6" t="s">
         <v>304</v>
       </c>
@@ -17301,7 +17335,7 @@
       </c>
       <c r="H350" s="8"/>
     </row>
-    <row r="351" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="351" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A351" s="6" t="s">
         <v>276</v>
       </c>
@@ -17322,7 +17356,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="352" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="352" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A352" s="6" t="s">
         <v>355</v>
       </c>
@@ -17343,7 +17377,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="353" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="353" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A353" s="6" t="s">
         <v>385</v>
       </c>
@@ -17364,7 +17398,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="354" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="354" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A354" s="6" t="s">
         <v>389</v>
       </c>
@@ -17387,7 +17421,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="355" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="355" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A355" s="6" t="s">
         <v>392</v>
       </c>
@@ -17408,7 +17442,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="356" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="356" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A356" s="6" t="s">
         <v>393</v>
       </c>
@@ -17429,7 +17463,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="357" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="357" spans="1:8" ht="46.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A357" s="6" t="s">
         <v>386</v>
       </c>
@@ -17452,7 +17486,7 @@
       </c>
       <c r="H357" s="8"/>
     </row>
-    <row r="358" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="358" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A358" s="6" t="s">
         <v>68</v>
       </c>
@@ -17475,7 +17509,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="359" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="359" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A359" s="6" t="s">
         <v>394</v>
       </c>
@@ -17496,7 +17530,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="360" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="360" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A360" s="6" t="s">
         <v>180</v>
       </c>
@@ -17517,7 +17551,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="361" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="361" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A361" s="6" t="s">
         <v>406</v>
       </c>
@@ -17538,7 +17572,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="362" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="362" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A362" s="6" t="s">
         <v>407</v>
       </c>
@@ -17559,7 +17593,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="363" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="363" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A363" s="6" t="s">
         <v>396</v>
       </c>
@@ -17580,7 +17614,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="364" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="364" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A364" s="6" t="s">
         <v>397</v>
       </c>
@@ -17601,7 +17635,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="365" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="365" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A365" s="6" t="s">
         <v>398</v>
       </c>
@@ -17622,7 +17656,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="366" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="366" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A366" s="6" t="s">
         <v>399</v>
       </c>
@@ -17643,7 +17677,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="367" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="367" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A367" s="6" t="s">
         <v>404</v>
       </c>
@@ -17664,7 +17698,7 @@
       <c r="G367" s="8"/>
       <c r="H367" s="8"/>
     </row>
-    <row r="368" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="368" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A368" s="6" t="s">
         <v>405</v>
       </c>
@@ -17685,7 +17719,7 @@
       <c r="G368" s="8"/>
       <c r="H368" s="8"/>
     </row>
-    <row r="369" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="369" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A369" s="6" t="s">
         <v>409</v>
       </c>
@@ -17706,7 +17740,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="370" spans="1:8" ht="63" x14ac:dyDescent="0.5">
+    <row r="370" spans="1:8" ht="62.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A370" s="6" t="s">
         <v>411</v>
       </c>
@@ -17729,7 +17763,7 @@
       </c>
       <c r="H370" s="8"/>
     </row>
-    <row r="371" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="371" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A371" s="6" t="s">
         <v>412</v>
       </c>
@@ -17750,7 +17784,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="372" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="372" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A372" s="6" t="s">
         <v>71</v>
       </c>
@@ -17771,7 +17805,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="373" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="373" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A373" s="6" t="s">
         <v>491</v>
       </c>
@@ -17792,7 +17826,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="374" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="374" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A374" s="6" t="s">
         <v>66</v>
       </c>
@@ -17813,7 +17847,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="375" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="375" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A375" s="6" t="s">
         <v>418</v>
       </c>
@@ -17834,7 +17868,7 @@
         <v>1109</v>
       </c>
     </row>
-    <row r="376" spans="1:8" ht="63" x14ac:dyDescent="0.5">
+    <row r="376" spans="1:8" ht="62.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A376" s="6" t="s">
         <v>419</v>
       </c>
@@ -17857,7 +17891,7 @@
       </c>
       <c r="H376" s="8"/>
     </row>
-    <row r="377" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="377" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A377" s="6" t="s">
         <v>420</v>
       </c>
@@ -17878,7 +17912,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="378" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="378" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A378" s="6" t="s">
         <v>422</v>
       </c>
@@ -17899,7 +17933,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="379" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="379" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A379" s="6" t="s">
         <v>415</v>
       </c>
@@ -17920,7 +17954,7 @@
         <v>1109</v>
       </c>
     </row>
-    <row r="380" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="380" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A380" s="6" t="s">
         <v>417</v>
       </c>
@@ -17941,7 +17975,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="381" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="381" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A381" s="6" t="s">
         <v>421</v>
       </c>
@@ -17962,7 +17996,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="382" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="382" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A382" s="6" t="s">
         <v>423</v>
       </c>
@@ -17983,7 +18017,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="383" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="383" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A383" s="6" t="s">
         <v>210</v>
       </c>
@@ -18004,7 +18038,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="384" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="384" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A384" s="6" t="s">
         <v>395</v>
       </c>
@@ -18025,7 +18059,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="385" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="385" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A385" s="6" t="s">
         <v>426</v>
       </c>
@@ -18046,7 +18080,7 @@
       </c>
       <c r="H385" s="8"/>
     </row>
-    <row r="386" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="386" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A386" s="6" t="s">
         <v>429</v>
       </c>
@@ -18067,7 +18101,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="387" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="387" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A387" s="6" t="s">
         <v>427</v>
       </c>
@@ -18088,7 +18122,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="388" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="388" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A388" s="6" t="s">
         <v>428</v>
       </c>
@@ -18109,7 +18143,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="389" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="389" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A389" s="6" t="s">
         <v>431</v>
       </c>
@@ -18130,7 +18164,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="390" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="390" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A390" s="6" t="s">
         <v>432</v>
       </c>
@@ -18151,7 +18185,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="391" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="391" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A391" s="6" t="s">
         <v>433</v>
       </c>
@@ -18172,7 +18206,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="392" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="392" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A392" s="6" t="s">
         <v>130</v>
       </c>
@@ -18193,7 +18227,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="393" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="393" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A393" s="6" t="s">
         <v>482</v>
       </c>
@@ -18214,7 +18248,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="394" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="394" spans="1:8" ht="46.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A394" s="6" t="s">
         <v>434</v>
       </c>
@@ -18235,7 +18269,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="395" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="395" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A395" s="6" t="s">
         <v>436</v>
       </c>
@@ -18258,7 +18292,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="396" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="396" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A396" s="6" t="s">
         <v>454</v>
       </c>
@@ -18279,7 +18313,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="397" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="397" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A397" s="6" t="s">
         <v>455</v>
       </c>
@@ -18300,7 +18334,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="398" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="398" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A398" s="6" t="s">
         <v>466</v>
       </c>
@@ -18321,7 +18355,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="399" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="399" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A399" s="6" t="s">
         <v>443</v>
       </c>
@@ -18342,7 +18376,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="400" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="400" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A400" s="6" t="s">
         <v>444</v>
       </c>
@@ -18363,7 +18397,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="401" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="401" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A401" s="6" t="s">
         <v>445</v>
       </c>
@@ -18384,7 +18418,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="402" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="402" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A402" s="6" t="s">
         <v>116</v>
       </c>
@@ -18405,7 +18439,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="403" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="403" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A403" s="6" t="s">
         <v>117</v>
       </c>
@@ -18426,7 +18460,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="404" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="404" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A404" s="6" t="s">
         <v>118</v>
       </c>
@@ -18447,7 +18481,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="405" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="405" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A405" s="6" t="s">
         <v>437</v>
       </c>
@@ -18468,7 +18502,7 @@
       <c r="G405" s="8"/>
       <c r="H405" s="8"/>
     </row>
-    <row r="406" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="406" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A406" s="6" t="s">
         <v>438</v>
       </c>
@@ -18489,7 +18523,7 @@
       <c r="G406" s="8"/>
       <c r="H406" s="8"/>
     </row>
-    <row r="407" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="407" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A407" s="6" t="s">
         <v>440</v>
       </c>
@@ -18510,7 +18544,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="408" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="408" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A408" s="6" t="s">
         <v>441</v>
       </c>
@@ -18531,7 +18565,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="409" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="409" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A409" s="6" t="s">
         <v>442</v>
       </c>
@@ -18552,7 +18586,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="410" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="410" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A410" s="6" t="s">
         <v>446</v>
       </c>
@@ -18573,7 +18607,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="411" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="411" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A411" s="6" t="s">
         <v>296</v>
       </c>
@@ -18594,7 +18628,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="412" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="412" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A412" s="6" t="s">
         <v>425</v>
       </c>
@@ -18615,7 +18649,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="413" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="413" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A413" s="6" t="s">
         <v>447</v>
       </c>
@@ -18636,7 +18670,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="414" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="414" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A414" s="6" t="s">
         <v>75</v>
       </c>
@@ -18657,7 +18691,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="415" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="415" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A415" s="6" t="s">
         <v>448</v>
       </c>
@@ -18678,7 +18712,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="416" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="416" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A416" s="6" t="s">
         <v>451</v>
       </c>
@@ -18699,7 +18733,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="417" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="417" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A417" s="6" t="s">
         <v>450</v>
       </c>
@@ -18720,7 +18754,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="418" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="418" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A418" s="6" t="s">
         <v>449</v>
       </c>
@@ -18741,7 +18775,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="419" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="419" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A419" s="6" t="s">
         <v>456</v>
       </c>
@@ -18762,7 +18796,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="420" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="420" spans="1:8" ht="46.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A420" s="6" t="s">
         <v>461</v>
       </c>
@@ -18783,7 +18817,7 @@
       </c>
       <c r="H420" s="8"/>
     </row>
-    <row r="421" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="421" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A421" s="6" t="s">
         <v>467</v>
       </c>
@@ -18804,7 +18838,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="422" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="422" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A422" s="6" t="s">
         <v>468</v>
       </c>
@@ -18825,7 +18859,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="423" spans="1:8" ht="63" x14ac:dyDescent="0.5">
+    <row r="423" spans="1:8" ht="62.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A423" s="6" t="s">
         <v>439</v>
       </c>
@@ -18846,7 +18880,7 @@
       </c>
       <c r="H423" s="8"/>
     </row>
-    <row r="424" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="424" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A424" s="6" t="s">
         <v>80</v>
       </c>
@@ -18867,7 +18901,7 @@
       </c>
       <c r="H424" s="8"/>
     </row>
-    <row r="425" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="425" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A425" s="6" t="s">
         <v>12</v>
       </c>
@@ -18888,7 +18922,7 @@
       <c r="G425" s="8"/>
       <c r="H425" s="8"/>
     </row>
-    <row r="426" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="426" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A426" s="6" t="s">
         <v>335</v>
       </c>
@@ -18911,7 +18945,7 @@
       </c>
       <c r="H426" s="8"/>
     </row>
-    <row r="427" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="427" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A427" s="6" t="s">
         <v>470</v>
       </c>
@@ -18932,7 +18966,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="428" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="428" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A428" s="6" t="s">
         <v>469</v>
       </c>
@@ -18953,7 +18987,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="429" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="429" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A429" s="6" t="s">
         <v>336</v>
       </c>
@@ -18974,7 +19008,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="430" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="430" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A430" s="6" t="s">
         <v>337</v>
       </c>
@@ -18995,7 +19029,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="431" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="431" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A431" s="6" t="s">
         <v>338</v>
       </c>
@@ -19016,7 +19050,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="432" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="432" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A432" s="6" t="s">
         <v>339</v>
       </c>
@@ -19037,7 +19071,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="433" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="433" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A433" s="6" t="s">
         <v>177</v>
       </c>
@@ -19058,7 +19092,7 @@
       </c>
       <c r="H433" s="8"/>
     </row>
-    <row r="434" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="434" spans="1:8" ht="46.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A434" s="6" t="s">
         <v>179</v>
       </c>
@@ -19079,7 +19113,7 @@
       </c>
       <c r="H434" s="8"/>
     </row>
-    <row r="435" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="435" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A435" s="6" t="s">
         <v>178</v>
       </c>
@@ -19100,7 +19134,7 @@
       </c>
       <c r="H435" s="8"/>
     </row>
-    <row r="436" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="436" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A436" s="6" t="s">
         <v>475</v>
       </c>
@@ -19121,7 +19155,7 @@
       <c r="G436" s="8"/>
       <c r="H436" s="8"/>
     </row>
-    <row r="437" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="437" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A437" s="6" t="s">
         <v>476</v>
       </c>
@@ -19142,7 +19176,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="438" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="438" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A438" s="6" t="s">
         <v>477</v>
       </c>
@@ -19163,7 +19197,7 @@
       <c r="G438" s="8"/>
       <c r="H438" s="8"/>
     </row>
-    <row r="439" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="439" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A439" s="6" t="s">
         <v>478</v>
       </c>
@@ -19184,7 +19218,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="440" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="440" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A440" s="6" t="s">
         <v>480</v>
       </c>
@@ -19205,7 +19239,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="441" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="441" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A441" s="6" t="s">
         <v>350</v>
       </c>
@@ -19226,7 +19260,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="442" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="442" spans="1:8" ht="46.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A442" s="6" t="s">
         <v>351</v>
       </c>
@@ -19247,7 +19281,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="443" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="443" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A443" s="6" t="s">
         <v>479</v>
       </c>
@@ -19268,7 +19302,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="444" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="444" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A444" s="6" t="s">
         <v>481</v>
       </c>
@@ -19289,7 +19323,7 @@
       </c>
       <c r="H444" s="8"/>
     </row>
-    <row r="445" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="445" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A445" s="6" t="s">
         <v>289</v>
       </c>
@@ -19310,7 +19344,7 @@
       </c>
       <c r="H445" s="8"/>
     </row>
-    <row r="446" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="446" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A446" s="6" t="s">
         <v>76</v>
       </c>
@@ -19331,7 +19365,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="447" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="447" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A447" s="6" t="s">
         <v>285</v>
       </c>
@@ -19352,7 +19386,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="448" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="448" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A448" s="6" t="s">
         <v>403</v>
       </c>
@@ -19373,7 +19407,7 @@
       </c>
       <c r="H448" s="8"/>
     </row>
-    <row r="449" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="449" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A449" s="6" t="s">
         <v>309</v>
       </c>
@@ -19394,7 +19428,7 @@
       </c>
       <c r="H449" s="8"/>
     </row>
-    <row r="450" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="450" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A450" s="6" t="s">
         <v>483</v>
       </c>
@@ -19415,7 +19449,7 @@
       </c>
       <c r="H450" s="8"/>
     </row>
-    <row r="451" spans="1:8" ht="78.75" x14ac:dyDescent="0.5">
+    <row r="451" spans="1:8" ht="78" hidden="1" x14ac:dyDescent="0.3">
       <c r="A451" s="6" t="s">
         <v>65</v>
       </c>
@@ -19436,7 +19470,7 @@
       </c>
       <c r="H451" s="8"/>
     </row>
-    <row r="452" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="452" spans="1:8" ht="46.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A452" s="6" t="s">
         <v>464</v>
       </c>
@@ -19460,7 +19494,7 @@
       </c>
       <c r="H452" s="8"/>
     </row>
-    <row r="453" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="453" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A453" s="6" t="s">
         <v>363</v>
       </c>
@@ -19483,7 +19517,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="454" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="454" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A454" s="6" t="s">
         <v>484</v>
       </c>
@@ -19504,7 +19538,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="455" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="455" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A455" s="6" t="s">
         <v>424</v>
       </c>
@@ -19525,7 +19559,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="456" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="456" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A456" s="6" t="s">
         <v>139</v>
       </c>
@@ -19548,7 +19582,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="457" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="457" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A457" s="6" t="s">
         <v>487</v>
       </c>
@@ -19571,7 +19605,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="458" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="458" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A458" s="6" t="s">
         <v>488</v>
       </c>
@@ -19594,7 +19628,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="459" spans="1:8" ht="110.25" x14ac:dyDescent="0.5">
+    <row r="459" spans="1:8" ht="109.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A459" s="6" t="s">
         <v>215</v>
       </c>
@@ -19619,7 +19653,7 @@
       </c>
       <c r="H459" s="8"/>
     </row>
-    <row r="460" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="460" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A460" s="6" t="s">
         <v>216</v>
       </c>
@@ -19640,7 +19674,7 @@
       </c>
       <c r="H460" s="8"/>
     </row>
-    <row r="461" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="461" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A461" s="12" t="s">
         <v>217</v>
       </c>
@@ -19661,7 +19695,7 @@
       </c>
       <c r="H461" s="8"/>
     </row>
-    <row r="462" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="462" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A462" s="12" t="s">
         <v>218</v>
       </c>
@@ -19682,7 +19716,7 @@
       </c>
       <c r="H462" s="8"/>
     </row>
-    <row r="463" spans="1:8" ht="63" x14ac:dyDescent="0.5">
+    <row r="463" spans="1:8" ht="62.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A463" s="12" t="s">
         <v>473</v>
       </c>
@@ -19705,7 +19739,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="464" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="464" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A464" s="12" t="s">
         <v>474</v>
       </c>
@@ -19726,7 +19760,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="465" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="465" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A465" s="12" t="s">
         <v>383</v>
       </c>
@@ -19749,7 +19783,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="466" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="466" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A466" s="12" t="s">
         <v>485</v>
       </c>
@@ -19770,7 +19804,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="467" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="467" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A467" s="12" t="s">
         <v>262</v>
       </c>
@@ -19791,7 +19825,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="468" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="468" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A468" s="12" t="s">
         <v>413</v>
       </c>
@@ -19816,7 +19850,7 @@
       </c>
       <c r="H468" s="8"/>
     </row>
-    <row r="469" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="469" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A469" s="12" t="s">
         <v>414</v>
       </c>
@@ -19837,7 +19871,7 @@
       </c>
       <c r="H469" s="8"/>
     </row>
-    <row r="470" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="470" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A470" s="12" t="s">
         <v>209</v>
       </c>
@@ -19858,7 +19892,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="471" spans="1:8" ht="63" x14ac:dyDescent="0.5">
+    <row r="471" spans="1:8" ht="62.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A471" s="12" t="s">
         <v>493</v>
       </c>
@@ -19881,7 +19915,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="472" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="472" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A472" s="12" t="s">
         <v>496</v>
       </c>
@@ -19902,7 +19936,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="473" spans="1:8" ht="63" x14ac:dyDescent="0.5">
+    <row r="473" spans="1:8" ht="62.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A473" s="12" t="s">
         <v>494</v>
       </c>
@@ -19923,7 +19957,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="474" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="474" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A474" s="12" t="s">
         <v>169</v>
       </c>
@@ -19944,7 +19978,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="475" spans="1:8" ht="94.5" x14ac:dyDescent="0.5">
+    <row r="475" spans="1:8" ht="93.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A475" s="12" t="s">
         <v>497</v>
       </c>
@@ -19967,7 +20001,7 @@
       </c>
       <c r="H475" s="8"/>
     </row>
-    <row r="476" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="476" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A476" s="12" t="s">
         <v>495</v>
       </c>
@@ -19988,7 +20022,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="477" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="477" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A477" s="12" t="s">
         <v>89</v>
       </c>
@@ -20009,7 +20043,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="478" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="478" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A478" s="12" t="s">
         <v>90</v>
       </c>
@@ -20030,7 +20064,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="479" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="479" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A479" s="12" t="s">
         <v>331</v>
       </c>
@@ -20051,7 +20085,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="480" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="480" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A480" s="12" t="s">
         <v>56</v>
       </c>
@@ -20072,7 +20106,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="481" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="481" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A481" s="12" t="s">
         <v>390</v>
       </c>
@@ -20093,7 +20127,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="482" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="482" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A482" s="12" t="s">
         <v>492</v>
       </c>
@@ -20114,7 +20148,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="483" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="483" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A483" s="12" t="s">
         <v>67</v>
       </c>
@@ -20135,7 +20169,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="484" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="484" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A484" s="12" t="s">
         <v>452</v>
       </c>
@@ -20156,7 +20190,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="485" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="485" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A485" s="12" t="s">
         <v>453</v>
       </c>
@@ -20177,7 +20211,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="486" spans="1:8" ht="63" x14ac:dyDescent="0.5">
+    <row r="486" spans="1:8" ht="62.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A486" s="12" t="s">
         <v>378</v>
       </c>
@@ -20200,7 +20234,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="487" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="487" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A487" s="12" t="s">
         <v>249</v>
       </c>
@@ -20221,7 +20255,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="488" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="488" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A488" s="12" t="s">
         <v>94</v>
       </c>
@@ -20242,7 +20276,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="489" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="489" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A489" s="12" t="s">
         <v>92</v>
       </c>
@@ -20263,7 +20297,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="490" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="490" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A490" s="12" t="s">
         <v>93</v>
       </c>
@@ -20284,7 +20318,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="491" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="491" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A491" s="12" t="s">
         <v>91</v>
       </c>
@@ -20305,7 +20339,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="492" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="492" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A492" s="12" t="s">
         <v>96</v>
       </c>
@@ -20326,7 +20360,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="493" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="493" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A493" s="12" t="s">
         <v>95</v>
       </c>
@@ -20347,7 +20381,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="494" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="494" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A494" s="12" t="s">
         <v>250</v>
       </c>
@@ -20368,7 +20402,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="495" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="495" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A495" s="12" t="s">
         <v>391</v>
       </c>
@@ -20389,7 +20423,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="496" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="496" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A496" s="12" t="s">
         <v>504</v>
       </c>
@@ -20412,7 +20446,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="497" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="497" spans="1:8" ht="46.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A497" s="12" t="s">
         <v>374</v>
       </c>
@@ -20435,7 +20469,7 @@
       </c>
       <c r="H497" s="8"/>
     </row>
-    <row r="498" spans="1:8" ht="63" x14ac:dyDescent="0.5">
+    <row r="498" spans="1:8" ht="62.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A498" s="12" t="s">
         <v>373</v>
       </c>
@@ -20456,7 +20490,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="499" spans="1:8" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="499" spans="1:8" ht="46.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A499" s="12" t="s">
         <v>372</v>
       </c>
@@ -20479,7 +20513,7 @@
       </c>
       <c r="H499" s="8"/>
     </row>
-    <row r="500" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="500" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A500" s="12" t="s">
         <v>457</v>
       </c>
@@ -20502,7 +20536,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="501" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="501" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A501" s="12" t="s">
         <v>458</v>
       </c>
@@ -20525,7 +20559,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="502" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="502" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A502" s="12" t="s">
         <v>190</v>
       </c>
@@ -20546,7 +20580,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="503" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="503" spans="1:8" ht="31.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A503" s="12" t="s">
         <v>191</v>
       </c>
@@ -20567,7 +20601,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="504" spans="1:8" ht="63" x14ac:dyDescent="0.5">
+    <row r="504" spans="1:8" ht="62.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A504" s="12" t="s">
         <v>163</v>
       </c>
@@ -20590,7 +20624,7 @@
       </c>
       <c r="H504" s="8"/>
     </row>
-    <row r="505" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="505" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A505" s="12" t="s">
         <v>329</v>
       </c>

</xml_diff>